<commit_message>
Added Test Case and data for User Management AddUser Special characters.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918FDD50-F978-4D51-BDF0-363755641856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CFEE84-1574-4AD0-B4DF-D0FA1BE63B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19350" yWindow="2355" windowWidth="17670" windowHeight="13890" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="4080" yWindow="2535" windowWidth="17670" windowHeight="13890" activeTab="3" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateUserSpCharError" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateUserSpChar" sheetId="3" r:id="rId3"/>
+    <sheet name="CaseUsername" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="28">
   <si>
     <t>Result</t>
   </si>
@@ -86,6 +89,39 @@
   </si>
   <si>
     <t>hello5555</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>@</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>CASEuser</t>
+  </si>
+  <si>
+    <t>caseuser</t>
+  </si>
+  <si>
+    <t>CASEUSER</t>
+  </si>
+  <si>
+    <t>hello2222</t>
   </si>
 </sst>
 </file>
@@ -136,12 +172,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:J4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,4 +616,346 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E3BA90D-A423-4791-B1FE-1A0581FBA0B0}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Custom Logger and Username not case sensitive Test case and data.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CFEE84-1574-4AD0-B4DF-D0FA1BE63B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1E87DB-BDFA-48E3-9379-FDDD69E18FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="2535" windowWidth="17670" windowHeight="13890" activeTab="3" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="4080" yWindow="2535" windowWidth="17670" windowHeight="13890" firstSheet="1" activeTab="3" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
     <sheet name="CreateUserSpCharError" sheetId="2" r:id="rId2"/>
     <sheet name="CreateUserSpChar" sheetId="3" r:id="rId3"/>
-    <sheet name="CaseUsername" sheetId="4" r:id="rId4"/>
+    <sheet name="UsernameCase" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -172,15 +172,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,11 +872,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E3BA90D-A423-4791-B1FE-1A0581FBA0B0}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,17 +885,12 @@
     <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -918,7 +910,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
@@ -928,9 +920,8 @@
       <c r="F2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -940,9 +931,8 @@
       <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
@@ -952,7 +942,6 @@
       <c r="F4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Test Cases and data for FindUser.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1E87DB-BDFA-48E3-9379-FDDD69E18FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEACF7F-C285-4BD2-90D2-3844571B9025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="2535" windowWidth="17670" windowHeight="13890" firstSheet="1" activeTab="3" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="-19200" yWindow="2400" windowWidth="17670" windowHeight="13890" firstSheet="2" activeTab="5" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
     <sheet name="CreateUserSpCharError" sheetId="2" r:id="rId2"/>
     <sheet name="CreateUserSpChar" sheetId="3" r:id="rId3"/>
     <sheet name="UsernameCase" sheetId="5" r:id="rId4"/>
+    <sheet name="PassCase" sheetId="6" r:id="rId5"/>
+    <sheet name="FindUser" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="46">
   <si>
     <t>Result</t>
   </si>
@@ -122,6 +124,60 @@
   </si>
   <si>
     <t>hello2222</t>
+  </si>
+  <si>
+    <t>HELLO2222</t>
+  </si>
+  <si>
+    <t>SearchType</t>
+  </si>
+  <si>
+    <t>chragui</t>
+  </si>
+  <si>
+    <t>Exact Match</t>
+  </si>
+  <si>
+    <t>Starts With</t>
+  </si>
+  <si>
+    <t>Ends With</t>
+  </si>
+  <si>
+    <t>Contains</t>
+  </si>
+  <si>
+    <t>Christinado</t>
+  </si>
+  <si>
+    <t>Aguillerezo</t>
+  </si>
+  <si>
+    <t>chra</t>
+  </si>
+  <si>
+    <t>agui</t>
+  </si>
+  <si>
+    <t>hragu</t>
+  </si>
+  <si>
+    <t>Christin</t>
+  </si>
+  <si>
+    <t>ristinado</t>
+  </si>
+  <si>
+    <t>hristina</t>
+  </si>
+  <si>
+    <t>Aguille</t>
+  </si>
+  <si>
+    <t>uillerezo</t>
+  </si>
+  <si>
+    <t>uillere</t>
   </si>
 </sst>
 </file>
@@ -495,7 +551,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,4 +1003,245 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="19.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Test Cases and Data for User Management User Errors.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEACF7F-C285-4BD2-90D2-3844571B9025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50221576-F8BB-4237-BC86-BC8A549712CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19200" yWindow="2400" windowWidth="17670" windowHeight="13890" firstSheet="2" activeTab="5" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="17670" windowHeight="13890" firstSheet="4" activeTab="8" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
     <sheet name="CreateUserSpCharError" sheetId="2" r:id="rId2"/>
-    <sheet name="CreateUserSpChar" sheetId="3" r:id="rId3"/>
-    <sheet name="UsernameCase" sheetId="5" r:id="rId4"/>
-    <sheet name="PassCase" sheetId="6" r:id="rId5"/>
-    <sheet name="FindUser" sheetId="7" r:id="rId6"/>
+    <sheet name="CreateUserSCFNameErr" sheetId="9" r:id="rId3"/>
+    <sheet name="CreateUserSCLNameErr" sheetId="10" r:id="rId4"/>
+    <sheet name="CreateUserSpChar" sheetId="3" r:id="rId5"/>
+    <sheet name="UsernameCase" sheetId="5" r:id="rId6"/>
+    <sheet name="PassCase" sheetId="6" r:id="rId7"/>
+    <sheet name="FindUser" sheetId="7" r:id="rId8"/>
+    <sheet name="CreateUserErrors" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="56">
   <si>
     <t>Result</t>
   </si>
@@ -178,6 +181,36 @@
   </si>
   <si>
     <t>uillere</t>
+  </si>
+  <si>
+    <t>abc@abc</t>
+  </si>
+  <si>
+    <t>abc.com</t>
+  </si>
+  <si>
+    <t>ErrorMsg</t>
+  </si>
+  <si>
+    <t>Email address is invalid</t>
+  </si>
+  <si>
+    <t>hello6666</t>
+  </si>
+  <si>
+    <t>please confirm the password for the new account</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Username is not unique</t>
   </si>
 </sst>
 </file>
@@ -551,7 +584,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection sqref="A1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +709,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD27"/>
+      <selection sqref="A1:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,6 +869,144 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="14.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -927,7 +1098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -1005,12 +1176,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,11 +1232,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -1244,4 +1415,189 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="47.5703125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Username and Password for Demo App 1773.  Changed VSP Submit button Object Repository properties.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31159B44-FD04-4B62-8E0C-8F1057266EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35702C64-9831-40F8-9ECA-E5ED5AEF4A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="7" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="5" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,6 @@
     <t>CASEUSER</t>
   </si>
   <si>
-    <t>hello2222</t>
-  </si>
-  <si>
     <t>HELLO2222</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>Username is not unique</t>
+  </si>
+  <si>
+    <t>Hello@2222</t>
   </si>
 </sst>
 </file>
@@ -261,12 +261,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,6 +702,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -865,6 +869,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -935,6 +942,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1003,6 +1013,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1095,6 +1108,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1102,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,7 +1129,7 @@
     <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1144,8 +1160,8 @@
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>27</v>
+      <c r="F2" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1155,8 +1171,8 @@
       <c r="E3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
+      <c r="F3" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1166,13 +1182,16 @@
       <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>27</v>
+      <c r="F4" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1223,12 +1242,15 @@
         <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1236,7 +1258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1276,7 +1298,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1284,10 +1306,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1295,10 +1317,10 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1306,10 +1328,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1317,10 +1339,10 @@
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1328,10 +1350,10 @@
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1339,10 +1361,10 @@
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1350,10 +1372,10 @@
         <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1361,10 +1383,10 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1372,10 +1394,10 @@
         <v>11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1383,10 +1405,10 @@
         <v>11</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1394,10 +1416,10 @@
         <v>11</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1405,15 +1427,18 @@
         <v>11</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1477,7 +1502,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1485,16 +1510,16 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
@@ -1506,7 +1531,7 @@
         <v>14</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1514,16 +1539,16 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
@@ -1535,7 +1560,7 @@
         <v>14</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1543,13 +1568,13 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>13</v>
@@ -1558,13 +1583,13 @@
         <v>16</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1575,10 +1600,10 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>13</v>
@@ -1593,11 +1618,14 @@
         <v>14</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added QA2Profile to VSP_Profile_TestCases.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35702C64-9831-40F8-9ECA-E5ED5AEF4A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA13F05-13EB-4B0E-8516-30E0D159A60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="5" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="9" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,11 @@
     <sheet name="PassCase" sheetId="6" r:id="rId7"/>
     <sheet name="FindUser" sheetId="7" r:id="rId8"/>
     <sheet name="CreateUserErrors" sheetId="8" r:id="rId9"/>
+    <sheet name="TestForTyler" sheetId="11" r:id="rId10"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TestForTyler!$A$1:$A$41</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="101">
   <si>
     <t>Result</t>
   </si>
@@ -211,16 +215,157 @@
   </si>
   <si>
     <t>Hello@2222</t>
+  </si>
+  <si>
+    <t>OVK67648</t>
+  </si>
+  <si>
+    <t>xFu7Y4Yx2</t>
+  </si>
+  <si>
+    <t>ovk67648</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:10:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:10:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:10:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:10:52 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:11:30 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:11:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:11:52 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:12:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:12:12 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:12:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:12:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:12:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:12:53 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:13:03 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:13:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:14:19 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:14:29 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:14:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:14:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:15:00 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:15:11 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:15:20 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:15:30 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:16:08 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:16:17 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:16:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:16:36 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:16:48 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:16:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:17:08 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:17:17 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:17:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:18:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:18:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:18:53 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:19:04 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:19:14 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:19:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:20:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri May 12 21:20:40 EDT 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -261,13 +406,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,18 +734,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -705,6 +849,733 @@
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="16.28515625" style="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A41" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -718,19 +1589,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -885,9 +1756,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="4" width="9.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -958,7 +1829,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="14.85546875" style="1"/>
+    <col min="1" max="16384" width="14.85546875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1029,19 +1900,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1118,19 +1989,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1160,7 +2031,7 @@
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1171,7 +2042,7 @@
       <c r="E3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1182,7 +2053,7 @@
       <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1205,13 +2076,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1264,15 +2135,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="19.42578125" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1452,19 +2323,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="45.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="47.5703125" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="45.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="47.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed UM Create User Password to temp Password Policy of Upper case, lower case and Number.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA13F05-13EB-4B0E-8516-30E0D159A60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8D6BBD-D411-4FCC-A5AF-980B72ECBB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="9" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="-27540" yWindow="210" windowWidth="24480" windowHeight="17160" firstSheet="3" activeTab="8" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="100">
   <si>
     <t>Result</t>
   </si>
@@ -97,9 +97,6 @@
     <t>AN</t>
   </si>
   <si>
-    <t>hello5555</t>
-  </si>
-  <si>
     <t>=</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>Email address is invalid</t>
   </si>
   <si>
-    <t>hello6666</t>
-  </si>
-  <si>
     <t>please confirm the password for the new account</t>
   </si>
   <si>
@@ -350,6 +344,9 @@
   </si>
   <si>
     <t>Fri May 12 21:20:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>Hello5555</t>
   </si>
 </sst>
 </file>
@@ -729,7 +726,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,10 +791,10 @@
         <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
@@ -814,10 +811,10 @@
         <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
@@ -834,10 +831,10 @@
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
@@ -856,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,682 +890,682 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1618,7 +1615,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1650,7 +1647,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="2"/>
     </row>
@@ -1662,7 +1659,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -1674,7 +1671,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -1686,7 +1683,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5" s="2"/>
     </row>
@@ -1698,7 +1695,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="2"/>
     </row>
@@ -1710,7 +1707,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" s="2"/>
     </row>
@@ -1722,7 +1719,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I8" s="2"/>
     </row>
@@ -1734,7 +1731,7 @@
         <v>14</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -1783,7 +1780,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1791,7 +1788,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1799,7 +1796,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,7 +1804,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1823,7 +1820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -1854,7 +1851,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1862,7 +1859,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1870,7 +1867,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1878,7 +1875,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1929,7 +1926,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -1961,7 +1958,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" s="2"/>
     </row>
@@ -1973,7 +1970,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -2029,10 +2026,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,10 +2037,10 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2051,10 +2048,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2110,10 +2107,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2169,7 +2166,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2177,10 +2174,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2188,10 +2185,10 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2199,10 +2196,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2210,10 +2207,10 @@
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2221,10 +2218,10 @@
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2232,10 +2229,10 @@
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2243,10 +2240,10 @@
         <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2254,10 +2251,10 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2265,10 +2262,10 @@
         <v>11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2276,10 +2273,10 @@
         <v>11</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2287,10 +2284,10 @@
         <v>11</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2298,10 +2295,10 @@
         <v>11</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2317,8 +2314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2373,7 +2370,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2381,28 +2378,28 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2410,28 +2407,28 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2439,28 +2436,28 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2468,28 +2465,28 @@
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added and Updated Code and test data for IWP30.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8D6BBD-D411-4FCC-A5AF-980B72ECBB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420968CC-A933-4222-AACE-8087E63CB543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27540" yWindow="210" windowWidth="24480" windowHeight="17160" firstSheet="3" activeTab="8" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="2280" yWindow="165" windowWidth="24480" windowHeight="17160" firstSheet="2" activeTab="5" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
@@ -127,9 +127,6 @@
     <t>CASEUSER</t>
   </si>
   <si>
-    <t>HELLO2222</t>
-  </si>
-  <si>
     <t>SearchType</t>
   </si>
   <si>
@@ -347,6 +344,9 @@
   </si>
   <si>
     <t>Hello5555</t>
+  </si>
+  <si>
+    <t>HELLO@2222</t>
   </si>
 </sst>
 </file>
@@ -403,12 +403,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,10 +792,10 @@
         <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
@@ -811,10 +812,10 @@
         <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
@@ -831,10 +832,10 @@
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
@@ -890,682 +891,682 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1986,8 +1987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,7 +2030,7 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,7 +2041,7 @@
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2051,7 +2052,7 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2068,7 +2069,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,8 +2110,8 @@
       <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
+      <c r="F2" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2166,7 +2167,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2174,10 +2175,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2185,10 +2186,10 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2196,10 +2197,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2207,10 +2208,10 @@
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2218,10 +2219,10 @@
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2229,10 +2230,10 @@
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2240,10 +2241,10 @@
         <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2251,10 +2252,10 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2262,10 +2263,10 @@
         <v>11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2273,10 +2274,10 @@
         <v>11</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2284,10 +2285,10 @@
         <v>11</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2295,10 +2296,10 @@
         <v>11</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2314,8 +2315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2370,7 +2371,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2378,28 +2379,28 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2407,28 +2408,28 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2436,28 +2437,28 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2468,25 +2469,25 @@
         <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TestLogin Test case and data.  Added Admin Suite URL to Demo2Profile.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420968CC-A933-4222-AACE-8087E63CB543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47072DD-475C-48BF-98DE-0EB6AD25BD38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="165" windowWidth="24480" windowHeight="17160" firstSheet="2" activeTab="5" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="3" activeTab="10" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="FindUser" sheetId="7" r:id="rId8"/>
     <sheet name="CreateUserErrors" sheetId="8" r:id="rId9"/>
     <sheet name="TestForTyler" sheetId="11" r:id="rId10"/>
+    <sheet name="TestLogin" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TestForTyler!$A$1:$A$41</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="101">
   <si>
     <t>Result</t>
   </si>
@@ -347,6 +348,9 @@
   </si>
   <si>
     <t>HELLO@2222</t>
+  </si>
+  <si>
+    <t>Hello@5555555</t>
   </si>
 </sst>
 </file>
@@ -403,13 +407,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,7 +730,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I3" sqref="I3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,8 +743,8 @@
     <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
@@ -791,11 +794,11 @@
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>98</v>
+      <c r="I2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
+        <v>100</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
@@ -811,11 +814,11 @@
       <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>98</v>
+      <c r="I3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" t="s">
+        <v>100</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
@@ -831,11 +834,11 @@
       <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>98</v>
+      <c r="I4" t="s">
+        <v>100</v>
+      </c>
+      <c r="J4" t="s">
+        <v>100</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
@@ -855,7 +858,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,6 +1575,91 @@
   </sheetData>
   <autoFilter ref="A1:A41" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}"/>
   <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1987,7 +2075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -2110,7 +2198,7 @@
       <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added AddDeleteUserPasswordSpChar Test Casea and data.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,36 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECB5DF3-D9B2-4B35-BA51-0DE744050E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{674B1A45-5FB3-4380-9CD5-86869E21A864}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="3" activeTab="10" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView activeTab="11" firstSheet="4" windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
-    <sheet name="CreateUserSpCharError" sheetId="2" r:id="rId2"/>
-    <sheet name="CreateUserSCFNameErr" sheetId="9" r:id="rId3"/>
-    <sheet name="CreateUserSCLNameErr" sheetId="10" r:id="rId4"/>
-    <sheet name="CreateUserSpChar" sheetId="3" r:id="rId5"/>
-    <sheet name="UsernameCase" sheetId="5" r:id="rId6"/>
-    <sheet name="PassCase" sheetId="6" r:id="rId7"/>
-    <sheet name="FindUser" sheetId="7" r:id="rId8"/>
-    <sheet name="CreateUserErrors" sheetId="8" r:id="rId9"/>
-    <sheet name="TestForTyler" sheetId="11" r:id="rId10"/>
-    <sheet name="TestLogin" sheetId="12" r:id="rId11"/>
+    <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
+    <sheet name="CreateUserSpCharError" r:id="rId2" sheetId="2"/>
+    <sheet name="CreateUserSCFNameErr" r:id="rId3" sheetId="9"/>
+    <sheet name="CreateUserSCLNameErr" r:id="rId4" sheetId="10"/>
+    <sheet name="CreateUserSpChar" r:id="rId5" sheetId="3"/>
+    <sheet name="UsernameCase" r:id="rId6" sheetId="5"/>
+    <sheet name="PassCase" r:id="rId7" sheetId="6"/>
+    <sheet name="FindUser" r:id="rId8" sheetId="7"/>
+    <sheet name="CreateUserErrors" r:id="rId9" sheetId="8"/>
+    <sheet name="TestForTyler" r:id="rId10" sheetId="11"/>
+    <sheet name="TestLogin" r:id="rId11" sheetId="12"/>
+    <sheet name="CreateUserPasswordSpChar" r:id="rId12" sheetId="13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TestForTyler!$A$1:$A$41</definedName>
+    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">TestForTyler!$A$1:$A$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="167">
   <si>
     <t>Result</t>
   </si>
@@ -351,12 +352,211 @@
   </si>
   <si>
     <t>Hello@5555555</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:15:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:15:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:16:15 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:16:29 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:16:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:17:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:17:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:17:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:17:48 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:18:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:18:16 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:18:30 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:18:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:19:00 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:19:15 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:19:29 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:19:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:19:57 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:20:20 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:20:44 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:21:09 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:21:29 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:21:44 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:21:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:22:14 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:22:30 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:22:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:22:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:23:14 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 29 09:23:28 EDT 2023</t>
+  </si>
+  <si>
+    <t>PasswordLength</t>
+  </si>
+  <si>
+    <t>PasswordSpChar</t>
+  </si>
+  <si>
+    <t>Create User with Special Characters in Password</t>
+  </si>
+  <si>
+    <t>!Aa1</t>
+  </si>
+  <si>
+    <t>@Bb2</t>
+  </si>
+  <si>
+    <t>#Cc3</t>
+  </si>
+  <si>
+    <t>$Dd4</t>
+  </si>
+  <si>
+    <t>%Ee5</t>
+  </si>
+  <si>
+    <t>^Ff6</t>
+  </si>
+  <si>
+    <t>&amp;Gg7</t>
+  </si>
+  <si>
+    <t>*Hh8</t>
+  </si>
+  <si>
+    <t>!Ii9</t>
+  </si>
+  <si>
+    <t>@Jj0</t>
+  </si>
+  <si>
+    <t>#Kk1</t>
+  </si>
+  <si>
+    <t>$Ll2</t>
+  </si>
+  <si>
+    <t>%Mm3</t>
+  </si>
+  <si>
+    <t>^Nn4</t>
+  </si>
+  <si>
+    <t>&amp;Oo5</t>
+  </si>
+  <si>
+    <t>*Pp5</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:39:01 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:39:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:40:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:40:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:41:03 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:41:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:42:00 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:42:28 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:42:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:43:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:43:53 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:44:22 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:44:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:45:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:45:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:46:14 EDT 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,20 +605,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -435,10 +638,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -473,7 +676,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -525,7 +728,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -636,21 +839,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -667,7 +870,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -719,15 +922,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3:J3"/>
@@ -735,18 +938,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -845,8 +1048,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -854,8 +1057,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
-  <dimension ref="A1:F41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -863,13 +1066,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="16.28515625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1575,24 +1778,24 @@
   </sheetData>
   <autoFilter ref="A1:A41" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1610,164 +1813,740 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>105</v>
+      </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>108</v>
+      </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>109</v>
+      </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>113</v>
+      </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>116</v>
+      </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>117</v>
+      </c>
       <c r="D18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>118</v>
+      </c>
       <c r="D19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
       <c r="D20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>120</v>
+      </c>
       <c r="D21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>121</v>
+      </c>
       <c r="D22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>122</v>
+      </c>
       <c r="D23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>123</v>
+      </c>
       <c r="D24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
       <c r="D25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
       <c r="D26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>126</v>
+      </c>
       <c r="D27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>127</v>
+      </c>
       <c r="D28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>128</v>
+      </c>
       <c r="D29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>129</v>
+      </c>
       <c r="D30" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" t="s">
+        <v>130</v>
+      </c>
       <c r="D31" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="28.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="38.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="21.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="21.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
+    <col min="14" max="16384" style="1" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row ht="30" r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" s="3">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row ht="30" r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="3">
+        <v>9</v>
+      </c>
+      <c r="J3" s="2"/>
+    </row>
+    <row ht="30" r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row ht="30" r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row ht="30" r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row ht="30" r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G7" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row ht="30" r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row ht="30" r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row ht="30" r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row ht="30" r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row ht="30" r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G12" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row ht="30" r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G13" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row ht="30" r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row ht="30" r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row ht="30" r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G16" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row ht="30" r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" s="3">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
-  <dimension ref="A1:L9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:L9"/>
@@ -1775,19 +2554,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1925,7 +2704,7 @@
       <c r="I9" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1933,8 +2712,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E5"/>
@@ -1942,9 +2721,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="4" style="1" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1997,8 +2776,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2006,8 +2785,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -2015,7 +2794,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="14.85546875" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2068,8 +2847,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2077,28 +2856,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD19"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2164,7 +2943,7 @@
       <c r="I3" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2172,8 +2951,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
@@ -2181,13 +2960,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.140625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2244,8 +3023,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2253,8 +3032,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -2262,13 +3041,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2303,8 +3082,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2312,8 +3091,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
@@ -2321,15 +3100,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2491,8 +3270,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2500,8 +3279,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
@@ -2509,19 +3288,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="45.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="47.5703125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="45.5703125" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="47.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2679,8 +3458,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Added Test Cases and Data for Modify User.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{674B1A45-5FB3-4380-9CD5-86869E21A864}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{2BA13198-3F7E-4336-A95D-C20E8F3FC37C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="11" firstSheet="4" windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-120"/>
+    <workbookView activeTab="13" firstSheet="6" windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
@@ -25,6 +25,8 @@
     <sheet name="TestForTyler" r:id="rId10" sheetId="11"/>
     <sheet name="TestLogin" r:id="rId11" sheetId="12"/>
     <sheet name="CreateUserPasswordSpChar" r:id="rId12" sheetId="13"/>
+    <sheet name="ModifyUser" r:id="rId13" sheetId="14"/>
+    <sheet name="ModifyUserPwd" r:id="rId14" sheetId="15"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">TestForTyler!$A$1:$A$41</definedName>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="189">
   <si>
     <t>Result</t>
   </si>
@@ -345,9 +347,6 @@
     <t>Fri May 12 21:20:40 EDT 2023</t>
   </si>
   <si>
-    <t>Hello5555</t>
-  </si>
-  <si>
     <t>HELLO@2222</t>
   </si>
   <si>
@@ -501,55 +500,124 @@
     <t>*Pp5</t>
   </si>
   <si>
+    <t>Sat Jul 01 21:39:01 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:39:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:40:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:40:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:41:03 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:41:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:42:00 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:42:28 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:42:56 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:43:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:43:53 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:44:22 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:44:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:45:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:45:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Sat Jul 01 21:46:14 EDT 2023</t>
+  </si>
+  <si>
+    <t>Hello@6666666</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 18:36:37 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 18:37:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 18:37:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 18:37:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>hello2222</t>
+  </si>
+  <si>
+    <t>Password does not match the Password Policy</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 20:23:01 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 20:23:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 20:28:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 20:29:00 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 20:29:29 EDT 2023</t>
+  </si>
+  <si>
+    <t>ToBeModUser</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Sat Jul 01 21:39:01 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:39:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:40:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:40:32 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:41:03 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:41:32 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:42:00 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:42:28 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:42:56 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:43:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:43:53 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:44:22 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:44:50 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:45:18 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:45:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:46:14 EDT 2023</t>
+    <t>Wed Jul 05 21:13:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 21:13:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 21:14:04 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 21:14:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 21:15:02 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 21:15:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 21:15:57 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 21:16:23 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 21:16:50 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jul 05 21:17:14 EDT 2023</t>
   </si>
 </sst>
 </file>
@@ -933,13 +1001,13 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J3"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
@@ -988,6 +1056,12 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
@@ -998,16 +1072,22 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>175</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1018,16 +1098,22 @@
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>176</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1038,10 +1124,10 @@
         <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
@@ -1817,7 +1903,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -1828,7 +1914,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1839,7 +1925,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -1850,7 +1936,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -1861,7 +1947,7 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1872,7 +1958,7 @@
         <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -1883,7 +1969,7 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -1894,7 +1980,7 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1905,7 +1991,7 @@
         <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -1916,7 +2002,7 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -1927,7 +2013,7 @@
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -1938,7 +2024,7 @@
         <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -1949,7 +2035,7 @@
         <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -1960,7 +2046,7 @@
         <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -1971,7 +2057,7 @@
         <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -1982,7 +2068,7 @@
         <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -1993,7 +2079,7 @@
         <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -2004,7 +2090,7 @@
         <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -2015,7 +2101,7 @@
         <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -2026,7 +2112,7 @@
         <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -2037,7 +2123,7 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -2048,7 +2134,7 @@
         <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -2059,7 +2145,7 @@
         <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -2070,7 +2156,7 @@
         <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -2081,7 +2167,7 @@
         <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -2092,7 +2178,7 @@
         <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -2103,7 +2189,7 @@
         <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -2114,7 +2200,7 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -2125,7 +2211,7 @@
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -2136,7 +2222,7 @@
         <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -2152,8 +2238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2191,10 +2277,10 @@
         <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -2220,16 +2306,16 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="G2" s="3">
         <v>9</v>
@@ -2241,16 +2327,16 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G3" s="3">
         <v>9</v>
@@ -2262,16 +2348,16 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G4" s="3">
         <v>9</v>
@@ -2282,16 +2368,16 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G5" s="3">
         <v>9</v>
@@ -2302,16 +2388,16 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G6" s="3">
         <v>9</v>
@@ -2322,16 +2408,16 @@
         <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G7" s="3">
         <v>9</v>
@@ -2342,16 +2428,16 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G8" s="3">
         <v>9</v>
@@ -2362,16 +2448,16 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G9" s="3">
         <v>9</v>
@@ -2382,16 +2468,16 @@
         <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G10" s="3">
         <v>10</v>
@@ -2402,16 +2488,16 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
@@ -2422,16 +2508,16 @@
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G12" s="3">
         <v>10</v>
@@ -2442,16 +2528,16 @@
         <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G13" s="3">
         <v>10</v>
@@ -2462,16 +2548,16 @@
         <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G14" s="3">
         <v>10</v>
@@ -2482,16 +2568,16 @@
         <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G15" s="3">
         <v>10</v>
@@ -2502,16 +2588,16 @@
         <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G16" s="3">
         <v>10</v>
@@ -2522,16 +2608,16 @@
         <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G17" s="3">
         <v>10</v>
@@ -2541,6 +2627,410 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J3" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J5" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J6" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J7" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J8" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J9" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J11" s="3">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -3078,7 +3568,7 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3095,7 +3585,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3280,24 +3770,24 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="13.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="20.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="45.5703125" collapsed="true"/>
     <col min="13" max="16384" style="1" width="47.5703125" collapsed="true"/>
@@ -3342,6 +3832,12 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
@@ -3357,11 +3853,11 @@
       <c r="H2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>98</v>
+      <c r="I2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" t="s">
+        <v>99</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
@@ -3371,6 +3867,12 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>167</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3386,11 +3888,11 @@
       <c r="H3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>98</v>
+      <c r="I3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" t="s">
+        <v>99</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
@@ -3400,6 +3902,12 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3415,11 +3923,11 @@
       <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>98</v>
+      <c r="I4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" t="s">
+        <v>165</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
@@ -3429,6 +3937,12 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>169</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3444,11 +3958,11 @@
       <c r="H5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>98</v>
+      <c r="I5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" t="s">
+        <v>99</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>14</v>
@@ -3456,6 +3970,69 @@
       <c r="L5" s="1" t="s">
         <v>51</v>
       </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6"/>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>170</v>
+      </c>
+      <c r="J6" t="s">
+        <v>170</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Updated User Management Test Cases and Data to add writing Test Results to Excel.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{2BA13198-3F7E-4336-A95D-C20E8F3FC37C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C20B6F-32AD-4FAC-9F8F-D573BF1FE65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="13" firstSheet="6" windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="8" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
-    <sheet name="CreateUserSpCharError" r:id="rId2" sheetId="2"/>
-    <sheet name="CreateUserSCFNameErr" r:id="rId3" sheetId="9"/>
-    <sheet name="CreateUserSCLNameErr" r:id="rId4" sheetId="10"/>
-    <sheet name="CreateUserSpChar" r:id="rId5" sheetId="3"/>
-    <sheet name="UsernameCase" r:id="rId6" sheetId="5"/>
-    <sheet name="PassCase" r:id="rId7" sheetId="6"/>
-    <sheet name="FindUser" r:id="rId8" sheetId="7"/>
-    <sheet name="CreateUserErrors" r:id="rId9" sheetId="8"/>
-    <sheet name="TestForTyler" r:id="rId10" sheetId="11"/>
-    <sheet name="TestLogin" r:id="rId11" sheetId="12"/>
-    <sheet name="CreateUserPasswordSpChar" r:id="rId12" sheetId="13"/>
-    <sheet name="ModifyUser" r:id="rId13" sheetId="14"/>
-    <sheet name="ModifyUserPwd" r:id="rId14" sheetId="15"/>
+    <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateUserSpCharError" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateUserSCFNameErr" sheetId="9" r:id="rId3"/>
+    <sheet name="CreateUserSCLNameErr" sheetId="10" r:id="rId4"/>
+    <sheet name="CreateUserSpChar" sheetId="3" r:id="rId5"/>
+    <sheet name="UsernameCase" sheetId="5" r:id="rId6"/>
+    <sheet name="PassCase" sheetId="6" r:id="rId7"/>
+    <sheet name="FindUser" sheetId="7" r:id="rId8"/>
+    <sheet name="CreateUserErrors" sheetId="8" r:id="rId9"/>
+    <sheet name="TestForTyler" sheetId="11" r:id="rId10"/>
+    <sheet name="TestLogin" sheetId="12" r:id="rId11"/>
+    <sheet name="CreateUserPasswordSpChar" sheetId="13" r:id="rId12"/>
+    <sheet name="ModifyUser" sheetId="14" r:id="rId13"/>
+    <sheet name="ModifyUserPwd" sheetId="15" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">TestForTyler!$A$1:$A$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TestForTyler!$A$1:$A$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="209">
   <si>
     <t>Result</t>
   </si>
@@ -587,9 +587,6 @@
     <t>ToBeModUser</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Wed Jul 05 21:13:02 EDT 2023</t>
   </si>
   <si>
@@ -618,13 +615,75 @@
   </si>
   <si>
     <t>Wed Jul 05 21:17:14 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 13:04:15 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 13:18:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 13:27:01 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 13:34:25 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 13:34:57 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 14:40:53 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 14:41:11 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 14:41:25 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 14:55:26 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 15:03:58 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 15:04:27 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 15:04:51 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 15:05:14 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 15:05:37 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 15:05:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 15:06:21 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 15:06:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 15:07:08 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 15:07:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 15:07:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jul 06 15:08:20 EDT 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -673,23 +732,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -706,10 +765,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -744,7 +803,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -796,7 +855,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -907,21 +966,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -938,7 +997,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -990,15 +1049,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
@@ -1006,18 +1065,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1134,8 +1193,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1143,8 +1202,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
-  <dimension ref="A1:G41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -1152,13 +1211,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="16.28515625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="16.28515625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1864,14 +1923,14 @@
   </sheetData>
   <autoFilter ref="A1:A41" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B11"/>
@@ -1879,9 +1938,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2229,14 +2288,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
-  <dimension ref="A1:N17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F11"/>
@@ -2244,20 +2303,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="28.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="38.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="21.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="21.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
-    <col min="14" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2301,7 +2360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -2322,7 +2381,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row ht="30" r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -2343,7 +2402,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row ht="30" r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -2363,7 +2422,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -2383,7 +2442,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2403,7 +2462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -2423,7 +2482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2443,7 +2502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2463,7 +2522,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -2483,7 +2542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2503,7 +2562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2523,7 +2582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2543,7 +2602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -2563,7 +2622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -2583,7 +2642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -2603,7 +2662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -2625,14 +2684,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -2640,18 +2699,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2742,29 +2801,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="22.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2804,7 +2863,7 @@
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -2827,7 +2886,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -2850,7 +2909,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -2873,7 +2932,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -2896,7 +2955,7 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -2919,7 +2978,7 @@
         <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -2942,7 +3001,7 @@
         <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -2965,7 +3024,7 @@
         <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -2988,7 +3047,7 @@
         <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -3011,7 +3070,7 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -3030,33 +3089,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
-  <dimension ref="A1:M9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L9"/>
+      <selection activeCell="D2" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3098,6 +3157,12 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>188</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
@@ -3194,7 +3259,7 @@
       <c r="I9" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3202,18 +3267,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" style="1" width="9.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.140625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3234,6 +3301,12 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
@@ -3266,8 +3339,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3275,16 +3348,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="1" width="14.85546875" collapsed="true"/>
+    <col min="1" max="16384" width="14.85546875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3305,6 +3378,12 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>190</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
@@ -3337,8 +3416,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3346,28 +3425,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3409,6 +3488,12 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>191</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
@@ -3421,6 +3506,12 @@
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>192</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3433,7 +3524,7 @@
       <c r="I3" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3441,22 +3532,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="22.140625" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3480,6 +3571,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>193</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
@@ -3491,6 +3588,12 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>194</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3502,6 +3605,12 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>195</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3513,8 +3622,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3522,8 +3631,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -3531,13 +3640,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3561,6 +3670,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>196</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
@@ -3572,8 +3687,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3581,24 +3696,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3628,6 +3743,12 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
@@ -3639,6 +3760,12 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>198</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3650,6 +3777,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>199</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3661,6 +3794,12 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>200</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3672,6 +3811,12 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>201</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3683,6 +3828,12 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>202</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3694,6 +3845,12 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>203</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
@@ -3705,6 +3862,12 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>204</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
@@ -3716,6 +3879,12 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>205</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
@@ -3727,6 +3896,12 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>206</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
@@ -3738,6 +3913,12 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>207</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
@@ -3749,6 +3930,12 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>208</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
@@ -3760,8 +3947,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3769,28 +3956,28 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
-  <dimension ref="A1:M17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="20.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="45.5703125" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="47.5703125" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="45.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="47.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4035,8 +4222,8 @@
       <c r="B17"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Minor changes to UM Test Data.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C20B6F-32AD-4FAC-9F8F-D573BF1FE65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EC4FDB-A94A-4924-A88B-0EC13C91E3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="8" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="1050" yWindow="1245" windowWidth="25455" windowHeight="13620" firstSheet="7" activeTab="8" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="233">
   <si>
     <t>Result</t>
   </si>
@@ -551,39 +551,15 @@
     <t>Hello@6666666</t>
   </si>
   <si>
-    <t>Wed Jul 05 18:36:37 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 18:37:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 18:37:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 18:37:50 EDT 2023</t>
-  </si>
-  <si>
     <t>hello2222</t>
   </si>
   <si>
-    <t>Password does not match the Password Policy</t>
-  </si>
-  <si>
     <t>Wed Jul 05 20:23:01 EDT 2023</t>
   </si>
   <si>
     <t>Wed Jul 05 20:23:42 EDT 2023</t>
   </si>
   <si>
-    <t>Wed Jul 05 20:28:27 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 20:29:00 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 20:29:29 EDT 2023</t>
-  </si>
-  <si>
     <t>ToBeModUser</t>
   </si>
   <si>
@@ -626,12 +602,6 @@
     <t>Thu Jul 06 13:27:01 EDT 2023</t>
   </si>
   <si>
-    <t>Thu Jul 06 13:34:25 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 13:34:57 EDT 2023</t>
-  </si>
-  <si>
     <t>Thu Jul 06 14:40:53 EDT 2023</t>
   </si>
   <si>
@@ -678,6 +648,108 @@
   </si>
   <si>
     <t>Thu Jul 06 15:08:20 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 21:26:37 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 21:27:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 21:27:34 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 21:30:10 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 21:30:40 EDT 2023</t>
+  </si>
+  <si>
+    <t>username236</t>
+  </si>
+  <si>
+    <t>Password is invalid</t>
+  </si>
+  <si>
+    <t>Hello@111111111111111111111111111</t>
+  </si>
+  <si>
+    <t>HELLO@1111111</t>
+  </si>
+  <si>
+    <t>hello@1111111</t>
+  </si>
+  <si>
+    <t>Hello@aaaaaaa</t>
+  </si>
+  <si>
+    <t>Hello1aaaaaaa</t>
+  </si>
+  <si>
+    <t>username238</t>
+  </si>
+  <si>
+    <t>username239</t>
+  </si>
+  <si>
+    <t>username240</t>
+  </si>
+  <si>
+    <t>username241</t>
+  </si>
+  <si>
+    <t>username242</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 22:19:19 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 22:19:43 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 22:20:04 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 22:20:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 22:20:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 22:21:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 22:21:53 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 22:22:15 EDT 2023</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 22:22:36 EDT 2023</t>
+  </si>
+  <si>
+    <t>username2370</t>
+  </si>
+  <si>
+    <t>Tue Sep 19 22:31:53 EDT 2023</t>
+  </si>
+  <si>
+    <t>Username@12345</t>
+  </si>
+  <si>
+    <t>Gorbachovaaaa@1</t>
+  </si>
+  <si>
+    <t>Password can not be the same as the username</t>
+  </si>
+  <si>
+    <t>Wed Sep 20 12:52:11 EDT 2023</t>
+  </si>
+  <si>
+    <t>First name can not contain</t>
+  </si>
+  <si>
+    <t>Wed Sep 20 12:54:35 EDT 2023</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1191,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -1145,7 +1217,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1171,7 +1243,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -2297,7 +2369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F11"/>
     </sheetView>
   </sheetViews>
@@ -2753,7 +2825,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -2779,7 +2851,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -2863,13 +2935,13 @@
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>28</v>
@@ -2886,13 +2958,13 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>28</v>
@@ -2909,13 +2981,13 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>28</v>
@@ -2932,13 +3004,13 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>28</v>
@@ -2955,13 +3027,13 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>28</v>
@@ -2978,13 +3050,13 @@
         <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>28</v>
@@ -3001,13 +3073,13 @@
         <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>28</v>
@@ -3024,13 +3096,13 @@
         <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>28</v>
@@ -3047,13 +3119,13 @@
         <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>28</v>
@@ -3070,13 +3142,13 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>28</v>
@@ -3161,7 +3233,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3305,7 +3377,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3382,7 +3454,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3492,7 +3564,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3510,7 +3582,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3575,7 +3647,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3592,7 +3664,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3609,7 +3681,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3674,7 +3746,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3747,7 +3819,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3764,7 +3836,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3781,7 +3853,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3798,7 +3870,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3815,7 +3887,7 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -3832,7 +3904,7 @@
         <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -3849,7 +3921,7 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -3866,7 +3938,7 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -3883,7 +3955,7 @@
         <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -3900,7 +3972,7 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -3917,7 +3989,7 @@
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -3934,7 +4006,7 @@
         <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -3960,7 +4032,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D2" sqref="D2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3969,12 +4041,12 @@
     <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="36" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="35.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="45.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="16384" width="47.5703125" style="1" collapsed="1"/>
@@ -4023,7 +4095,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>216</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -4058,7 +4130,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -4093,7 +4165,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>218</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -4125,10 +4197,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>219</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -4159,12 +4231,17 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6"/>
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>220</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
+        <v>204</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>48</v>
@@ -4176,38 +4253,262 @@
         <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7"/>
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8"/>
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>207</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9"/>
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>208</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10"/>
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>209</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11"/>
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12"/>
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>227</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>227</v>
+      </c>
+      <c r="J12" t="s">
+        <v>227</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13"/>
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>232</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F13" t="s">
+        <v>228</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" t="s">
+        <v>228</v>
+      </c>
+      <c r="J13" t="s">
+        <v>228</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14"/>
@@ -4222,6 +4523,7 @@
       <c r="B17"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
RAD Added 4 new Business Rep Fields to all Tax Forms except Personal.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EC4FDB-A94A-4924-A88B-0EC13C91E3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9D6B32-0EB9-4556-AD93-E5E3A9A75E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="1245" windowWidth="25455" windowHeight="13620" firstSheet="7" activeTab="8" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="7" activeTab="8" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="237">
   <si>
     <t>Result</t>
   </si>
@@ -698,9 +698,6 @@
     <t>username241</t>
   </si>
   <si>
-    <t>username242</t>
-  </si>
-  <si>
     <t>Tue Sep 19 22:19:19 EDT 2023</t>
   </si>
   <si>
@@ -749,14 +746,29 @@
     <t>First name can not contain</t>
   </si>
   <si>
-    <t>Wed Sep 20 12:54:35 EDT 2023</t>
+    <t>Gorbachovaaaa</t>
+  </si>
+  <si>
+    <t>username2431</t>
+  </si>
+  <si>
+    <t>Minjas</t>
+  </si>
+  <si>
+    <t>Fri Sep 22 15:16:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Fri Sep 22 15:16:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>username2436</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -766,6 +778,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -803,10 +823,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -815,8 +836,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4043,7 +4066,7 @@
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="18.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.5703125" style="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="36" style="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="35.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
@@ -4095,7 +4118,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -4130,7 +4153,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -4165,7 +4188,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -4200,7 +4223,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -4235,7 +4258,7 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -4270,13 +4293,13 @@
         <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>48</v>
@@ -4305,7 +4328,7 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -4340,7 +4363,7 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -4375,7 +4398,7 @@
         <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -4410,7 +4433,7 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -4445,13 +4468,13 @@
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>48</v>
@@ -4463,33 +4486,33 @@
         <v>13</v>
       </c>
       <c r="I12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="F13" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>49</v>
@@ -4497,21 +4520,53 @@
       <c r="H13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I13" t="s">
-        <v>228</v>
+      <c r="I13" s="4" t="s">
+        <v>227</v>
       </c>
       <c r="J13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L13" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F14" t="s">
+        <v>233</v>
+      </c>
+      <c r="G14" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14"/>
+      <c r="H14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" t="s">
+        <v>227</v>
+      </c>
+      <c r="J14" t="s">
+        <v>227</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15"/>
@@ -4524,8 +4579,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="I13" r:id="rId1" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updated RAD Test Cases and data to handle FEIN/SSN and Failures when Payment Applications are not deployed in QA2.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9D6B32-0EB9-4556-AD93-E5E3A9A75E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{654BFB58-3A8E-4969-A35C-1F52176A2ACC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="7" activeTab="8" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView activeTab="8" firstSheet="7" windowHeight="17640" windowWidth="29040" xWindow="-28920" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
-    <sheet name="CreateUserSpCharError" sheetId="2" r:id="rId2"/>
-    <sheet name="CreateUserSCFNameErr" sheetId="9" r:id="rId3"/>
-    <sheet name="CreateUserSCLNameErr" sheetId="10" r:id="rId4"/>
-    <sheet name="CreateUserSpChar" sheetId="3" r:id="rId5"/>
-    <sheet name="UsernameCase" sheetId="5" r:id="rId6"/>
-    <sheet name="PassCase" sheetId="6" r:id="rId7"/>
-    <sheet name="FindUser" sheetId="7" r:id="rId8"/>
-    <sheet name="CreateUserErrors" sheetId="8" r:id="rId9"/>
-    <sheet name="TestForTyler" sheetId="11" r:id="rId10"/>
-    <sheet name="TestLogin" sheetId="12" r:id="rId11"/>
-    <sheet name="CreateUserPasswordSpChar" sheetId="13" r:id="rId12"/>
-    <sheet name="ModifyUser" sheetId="14" r:id="rId13"/>
-    <sheet name="ModifyUserPwd" sheetId="15" r:id="rId14"/>
+    <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
+    <sheet name="CreateUserSpCharError" r:id="rId2" sheetId="2"/>
+    <sheet name="CreateUserSCFNameErr" r:id="rId3" sheetId="9"/>
+    <sheet name="CreateUserSCLNameErr" r:id="rId4" sheetId="10"/>
+    <sheet name="CreateUserSpChar" r:id="rId5" sheetId="3"/>
+    <sheet name="UsernameCase" r:id="rId6" sheetId="5"/>
+    <sheet name="PassCase" r:id="rId7" sheetId="6"/>
+    <sheet name="FindUser" r:id="rId8" sheetId="7"/>
+    <sheet name="CreateUserErrors" r:id="rId9" sheetId="8"/>
+    <sheet name="TestForTyler" r:id="rId10" sheetId="11"/>
+    <sheet name="TestLogin" r:id="rId11" sheetId="12"/>
+    <sheet name="CreateUserPasswordSpChar" r:id="rId12" sheetId="13"/>
+    <sheet name="ModifyUser" r:id="rId13" sheetId="14"/>
+    <sheet name="ModifyUserPwd" r:id="rId14" sheetId="15"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TestForTyler!$A$1:$A$41</definedName>
+    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">TestForTyler!$A$1:$A$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="241">
   <si>
     <t>Result</t>
   </si>
@@ -698,76 +698,89 @@
     <t>username241</t>
   </si>
   <si>
-    <t>Tue Sep 19 22:19:19 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 22:19:43 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 22:20:04 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 22:20:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 22:20:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 22:21:32 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 22:21:53 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 22:22:15 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 22:22:36 EDT 2023</t>
-  </si>
-  <si>
-    <t>username2370</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 22:31:53 EDT 2023</t>
-  </si>
-  <si>
-    <t>Username@12345</t>
-  </si>
-  <si>
     <t>Gorbachovaaaa@1</t>
   </si>
   <si>
     <t>Password can not be the same as the username</t>
   </si>
   <si>
-    <t>Wed Sep 20 12:52:11 EDT 2023</t>
-  </si>
-  <si>
-    <t>First name can not contain</t>
-  </si>
-  <si>
     <t>Gorbachovaaaa</t>
   </si>
   <si>
-    <t>username2431</t>
-  </si>
-  <si>
     <t>Minjas</t>
   </si>
   <si>
-    <t>Fri Sep 22 15:16:07 EDT 2023</t>
-  </si>
-  <si>
-    <t>Fri Sep 22 15:16:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>username2436</t>
+    <t>username2371</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 12:53:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 12:53:54 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 12:54:20 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 12:54:41 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 12:55:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 12:55:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 12:55:55 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 12:56:20 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 12:56:44 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 12:57:09 EDT 2023</t>
+  </si>
+  <si>
+    <t>Username@12347</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 13:40:32 EDT 2023</t>
+  </si>
+  <si>
+    <t>username2439</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 15:27:01 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 15:27:29 EDT 2023</t>
+  </si>
+  <si>
+    <t>username3001</t>
+  </si>
+  <si>
+    <t>Gorbachovaaaab</t>
+  </si>
+  <si>
+    <t>Gorbachovaaaab@1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Thu Sep 28 15:29:18 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Sep 28 15:29:45 EDT 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -824,26 +837,26 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -860,10 +873,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -898,7 +911,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -950,7 +963,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1061,21 +1074,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1092,7 +1105,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1144,15 +1157,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
@@ -1160,18 +1173,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1288,8 +1301,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1297,8 +1310,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
-  <dimension ref="A1:F41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -1306,13 +1319,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="16.28515625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2018,14 +2031,14 @@
   </sheetData>
   <autoFilter ref="A1:A41" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B11"/>
@@ -2033,9 +2046,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2383,14 +2396,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
-  <dimension ref="A1:M17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F11"/>
@@ -2398,20 +2411,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="28.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="38.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="21.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="21.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
+    <col min="14" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2455,7 +2468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -2476,7 +2489,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -2497,7 +2510,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -2517,7 +2530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -2537,7 +2550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2557,7 +2570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -2577,7 +2590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2597,7 +2610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2617,7 +2630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -2637,7 +2650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2657,7 +2670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2677,7 +2690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2697,7 +2710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -2717,7 +2730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -2737,7 +2750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -2757,7 +2770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -2779,14 +2792,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -2794,18 +2807,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2896,13 +2909,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
-  <dimension ref="A1:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
@@ -2910,15 +2923,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -3184,13 +3197,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
-  <dimension ref="A1:L9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D9"/>
@@ -3198,19 +3211,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3354,7 +3367,7 @@
       <c r="I9" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3362,8 +3375,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
@@ -3371,11 +3384,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="3" max="4" style="1" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3434,8 +3447,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3443,8 +3456,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
@@ -3452,7 +3465,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="14.85546875" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3511,8 +3524,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3520,8 +3533,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -3529,19 +3542,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3619,7 +3632,7 @@
       <c r="I3" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3627,8 +3640,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -3636,13 +3649,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.140625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3717,8 +3730,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3726,8 +3739,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -3735,13 +3748,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3782,8 +3795,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3791,8 +3804,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
@@ -3800,15 +3813,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4042,8 +4055,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4051,28 +4064,28 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
-  <dimension ref="A1:L17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D12"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="36" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="45.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="47.5703125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="36.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="35.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="45.5703125" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="47.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4118,10 +4131,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>220</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>50</v>
@@ -4153,10 +4163,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>221</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>50</v>
@@ -4188,10 +4195,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>222</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>50</v>
@@ -4223,10 +4227,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>218</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>223</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>23</v>
@@ -4258,10 +4259,7 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>224</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>204</v>
@@ -4295,11 +4293,8 @@
       <c r="B7" t="s">
         <v>225</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>48</v>
@@ -4328,10 +4323,7 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>220</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>226</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>211</v>
@@ -4363,10 +4355,7 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>227</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>212</v>
@@ -4398,10 +4387,7 @@
         <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
+        <v>228</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>213</v>
@@ -4433,10 +4419,7 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>229</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>214</v>
@@ -4468,13 +4451,10 @@
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>231</v>
       </c>
       <c r="E12" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>48</v>
@@ -4485,34 +4465,34 @@
       <c r="H12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I12" t="s">
-        <v>226</v>
-      </c>
-      <c r="J12" t="s">
-        <v>226</v>
+      <c r="I12" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F13" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>49</v>
@@ -4521,51 +4501,51 @@
         <v>13</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="J13" t="s">
-        <v>227</v>
+        <v>237</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F14" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="G14" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="J14" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -4580,10 +4560,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I13" r:id="rId1" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
+    <hyperlink r:id="rId1" ref="I13" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
+    <hyperlink r:id="rId2" ref="I12" xr:uid="{72B34BFC-1C06-4629-A7D1-00835E578F1C}"/>
+    <hyperlink r:id="rId3" ref="J12" xr:uid="{05843862-7C41-4D97-A198-1A33D27EECAF}"/>
+    <hyperlink r:id="rId4" ref="J13" xr:uid="{4B596713-18AE-4E73-886D-498F1C2E6C62}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId5" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Made changes to FEIN/SSN Object Identification.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{654BFB58-3A8E-4969-A35C-1F52176A2ACC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB401DB-C369-48E3-9BEA-1647B1D05DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="8" firstSheet="7" windowHeight="17640" windowWidth="29040" xWindow="-28920" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-120"/>
+    <workbookView xWindow="-20070" yWindow="1185" windowWidth="18810" windowHeight="14565" firstSheet="10" activeTab="13" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
-    <sheet name="CreateUserSpCharError" r:id="rId2" sheetId="2"/>
-    <sheet name="CreateUserSCFNameErr" r:id="rId3" sheetId="9"/>
-    <sheet name="CreateUserSCLNameErr" r:id="rId4" sheetId="10"/>
-    <sheet name="CreateUserSpChar" r:id="rId5" sheetId="3"/>
-    <sheet name="UsernameCase" r:id="rId6" sheetId="5"/>
-    <sheet name="PassCase" r:id="rId7" sheetId="6"/>
-    <sheet name="FindUser" r:id="rId8" sheetId="7"/>
-    <sheet name="CreateUserErrors" r:id="rId9" sheetId="8"/>
-    <sheet name="TestForTyler" r:id="rId10" sheetId="11"/>
-    <sheet name="TestLogin" r:id="rId11" sheetId="12"/>
-    <sheet name="CreateUserPasswordSpChar" r:id="rId12" sheetId="13"/>
-    <sheet name="ModifyUser" r:id="rId13" sheetId="14"/>
-    <sheet name="ModifyUserPwd" r:id="rId14" sheetId="15"/>
+    <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateUserSpCharError" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateUserSCFNameErr" sheetId="9" r:id="rId3"/>
+    <sheet name="CreateUserSCLNameErr" sheetId="10" r:id="rId4"/>
+    <sheet name="CreateUserSpChar" sheetId="3" r:id="rId5"/>
+    <sheet name="UsernameCase" sheetId="5" r:id="rId6"/>
+    <sheet name="PassCase" sheetId="6" r:id="rId7"/>
+    <sheet name="FindUser" sheetId="7" r:id="rId8"/>
+    <sheet name="CreateUserErrors" sheetId="8" r:id="rId9"/>
+    <sheet name="TestForTyler" sheetId="11" r:id="rId10"/>
+    <sheet name="TestLogin" sheetId="12" r:id="rId11"/>
+    <sheet name="CreateUserPasswordSpChar" sheetId="13" r:id="rId12"/>
+    <sheet name="ModifyUser" sheetId="14" r:id="rId13"/>
+    <sheet name="ModifyUserPwd" sheetId="15" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">TestForTyler!$A$1:$A$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TestForTyler!$A$1:$A$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="235">
   <si>
     <t>Result</t>
   </si>
@@ -563,36 +563,6 @@
     <t>ToBeModUser</t>
   </si>
   <si>
-    <t>Wed Jul 05 21:13:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 21:13:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 21:14:04 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 21:14:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 21:15:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 21:15:32 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 21:15:57 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 21:16:23 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 21:16:50 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 21:17:14 EDT 2023</t>
-  </si>
-  <si>
     <t>Thu Jul 06 13:04:15 EDT 2023</t>
   </si>
   <si>
@@ -752,12 +722,6 @@
     <t>username2439</t>
   </si>
   <si>
-    <t>Thu Sep 28 15:27:01 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Sep 28 15:27:29 EDT 2023</t>
-  </si>
-  <si>
     <t>username3001</t>
   </si>
   <si>
@@ -767,20 +731,37 @@
     <t>Gorbachovaaaab@1</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Thu Sep 28 15:29:18 EDT 2023</t>
   </si>
   <si>
     <t>Thu Sep 28 15:29:45 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Nov 01 13:59:13 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Nov 01 13:59:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Nov 01 14:00:10 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Nov 01 14:00:38 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Nov 01 14:01:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Nov 01 14:02:47 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Nov 01 14:03:12 EDT 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -837,26 +818,26 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -873,10 +854,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -911,7 +892,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -963,7 +944,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1074,21 +1055,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1105,7 +1086,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1157,15 +1138,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
@@ -1173,18 +1154,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1227,7 +1208,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -1253,7 +1234,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1279,7 +1260,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -1301,8 +1282,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1310,8 +1291,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
-  <dimension ref="A1:G41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -1319,13 +1300,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="16.28515625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="16.28515625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2031,14 +2012,14 @@
   </sheetData>
   <autoFilter ref="A1:A41" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B11"/>
@@ -2046,9 +2027,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2396,14 +2377,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
-  <dimension ref="A1:N17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F11"/>
@@ -2411,20 +2392,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="28.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="38.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="21.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="21.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
-    <col min="14" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2468,7 +2449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -2489,7 +2470,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row ht="30" r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -2510,7 +2491,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row ht="30" r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -2530,7 +2511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -2550,7 +2531,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2570,7 +2551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -2590,7 +2571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2610,7 +2591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2630,7 +2611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -2650,7 +2631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2670,7 +2651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2690,7 +2671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2710,7 +2691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -2730,7 +2711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -2750,7 +2731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -2770,7 +2751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -2792,14 +2773,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -2807,18 +2788,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2909,29 +2890,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="22.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2971,7 +2952,7 @@
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>228</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -2994,7 +2975,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>229</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3017,7 +2998,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>230</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3040,7 +3021,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>231</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3063,7 +3044,7 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>232</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -3086,7 +3067,7 @@
         <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>233</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -3098,7 +3079,7 @@
         <v>28</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="J7" s="3">
         <v>9</v>
@@ -3106,10 +3087,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>234</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -3121,89 +3102,20 @@
         <v>28</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J8" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J9" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" t="s">
-        <v>178</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="J10" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" t="s">
-        <v>179</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="J11" s="3">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
-  <dimension ref="A1:M9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D9"/>
@@ -3211,19 +3123,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3269,7 +3181,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3367,7 +3279,7 @@
       <c r="I9" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3375,8 +3287,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
@@ -3384,11 +3296,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="4" style="1" width="9.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.140625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3413,7 +3325,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3447,8 +3359,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3456,8 +3368,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
@@ -3465,7 +3377,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="1" width="14.85546875" collapsed="true"/>
+    <col min="1" max="16384" width="14.85546875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3490,7 +3402,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3524,8 +3436,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3533,8 +3445,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -3542,19 +3454,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3600,7 +3512,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3618,7 +3530,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3632,7 +3544,7 @@
       <c r="I3" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3640,8 +3552,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -3649,13 +3561,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="22.140625" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3683,7 +3595,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3700,7 +3612,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3717,7 +3629,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3730,8 +3642,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3739,8 +3651,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -3748,13 +3660,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3782,7 +3694,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3795,8 +3707,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3804,8 +3716,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
@@ -3813,15 +3725,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3855,7 +3767,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3872,7 +3784,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3889,7 +3801,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3906,7 +3818,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3923,7 +3835,7 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -3940,7 +3852,7 @@
         <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -3957,7 +3869,7 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -3974,7 +3886,7 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -3991,7 +3903,7 @@
         <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -4008,7 +3920,7 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -4025,7 +3937,7 @@
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -4042,7 +3954,7 @@
         <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -4055,8 +3967,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4064,28 +3976,28 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
-  <dimension ref="A1:M17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="36.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="35.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="45.5703125" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="47.5703125" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="36" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="35.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="45.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="47.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4131,7 +4043,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>50</v>
@@ -4163,7 +4075,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>50</v>
@@ -4195,7 +4107,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>50</v>
@@ -4227,7 +4139,7 @@
         <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>23</v>
@@ -4259,10 +4171,10 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>48</v>
@@ -4283,7 +4195,7 @@
         <v>14</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -4291,10 +4203,10 @@
         <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>48</v>
@@ -4306,16 +4218,16 @@
         <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="J7" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -4323,10 +4235,10 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>48</v>
@@ -4338,16 +4250,16 @@
         <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -4355,10 +4267,10 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>48</v>
@@ -4370,16 +4282,16 @@
         <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -4387,10 +4299,10 @@
         <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>48</v>
@@ -4402,16 +4314,16 @@
         <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -4419,10 +4331,10 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>48</v>
@@ -4434,16 +4346,16 @@
         <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -4451,10 +4363,10 @@
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E12" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>48</v>
@@ -4466,16 +4378,16 @@
         <v>13</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -4483,16 +4395,16 @@
         <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="F13" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>49</v>
@@ -4501,16 +4413,16 @@
         <v>13</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -4518,34 +4430,34 @@
         <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="F14" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G14" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="J14" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -4560,13 +4472,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="I13" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
-    <hyperlink r:id="rId2" ref="I12" xr:uid="{72B34BFC-1C06-4629-A7D1-00835E578F1C}"/>
-    <hyperlink r:id="rId3" ref="J12" xr:uid="{05843862-7C41-4D97-A198-1A33D27EECAF}"/>
-    <hyperlink r:id="rId4" ref="J13" xr:uid="{4B596713-18AE-4E73-886D-498F1C2E6C62}"/>
+    <hyperlink ref="I13" r:id="rId1" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
+    <hyperlink ref="I12" r:id="rId2" xr:uid="{72B34BFC-1C06-4629-A7D1-00835E578F1C}"/>
+    <hyperlink ref="J12" r:id="rId3" xr:uid="{05843862-7C41-4D97-A198-1A33D27EECAF}"/>
+    <hyperlink ref="J13" r:id="rId4" xr:uid="{4B596713-18AE-4E73-886D-498F1C2E6C62}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId5" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updated BBP-SelIDE Test Cases.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB401DB-C369-48E3-9BEA-1647B1D05DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{5FB401DB-C369-48E3-9BEA-1647B1D05DC1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-20070" yWindow="1185" windowWidth="18810" windowHeight="14565" firstSheet="10" activeTab="13" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView activeTab="13" firstSheet="10" windowHeight="14565" windowWidth="18810" xWindow="-20070" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="1185"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
-    <sheet name="CreateUserSpCharError" sheetId="2" r:id="rId2"/>
-    <sheet name="CreateUserSCFNameErr" sheetId="9" r:id="rId3"/>
-    <sheet name="CreateUserSCLNameErr" sheetId="10" r:id="rId4"/>
-    <sheet name="CreateUserSpChar" sheetId="3" r:id="rId5"/>
-    <sheet name="UsernameCase" sheetId="5" r:id="rId6"/>
-    <sheet name="PassCase" sheetId="6" r:id="rId7"/>
-    <sheet name="FindUser" sheetId="7" r:id="rId8"/>
-    <sheet name="CreateUserErrors" sheetId="8" r:id="rId9"/>
-    <sheet name="TestForTyler" sheetId="11" r:id="rId10"/>
-    <sheet name="TestLogin" sheetId="12" r:id="rId11"/>
-    <sheet name="CreateUserPasswordSpChar" sheetId="13" r:id="rId12"/>
-    <sheet name="ModifyUser" sheetId="14" r:id="rId13"/>
-    <sheet name="ModifyUserPwd" sheetId="15" r:id="rId14"/>
+    <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
+    <sheet name="CreateUserSpCharError" r:id="rId2" sheetId="2"/>
+    <sheet name="CreateUserSCFNameErr" r:id="rId3" sheetId="9"/>
+    <sheet name="CreateUserSCLNameErr" r:id="rId4" sheetId="10"/>
+    <sheet name="CreateUserSpChar" r:id="rId5" sheetId="3"/>
+    <sheet name="UsernameCase" r:id="rId6" sheetId="5"/>
+    <sheet name="PassCase" r:id="rId7" sheetId="6"/>
+    <sheet name="FindUser" r:id="rId8" sheetId="7"/>
+    <sheet name="CreateUserErrors" r:id="rId9" sheetId="8"/>
+    <sheet name="TestForTyler" r:id="rId10" sheetId="11"/>
+    <sheet name="TestLogin" r:id="rId11" sheetId="12"/>
+    <sheet name="CreateUserPasswordSpChar" r:id="rId12" sheetId="13"/>
+    <sheet name="ModifyUser" r:id="rId13" sheetId="14"/>
+    <sheet name="ModifyUserPwd" r:id="rId14" sheetId="15"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TestForTyler!$A$1:$A$41</definedName>
+    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">TestForTyler!$A$1:$A$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="240">
   <si>
     <t>Result</t>
   </si>
@@ -756,12 +756,28 @@
   </si>
   <si>
     <t>Wed Nov 01 14:03:12 EDT 2023</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Mon Nov 13 11:00:06 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Nov 13 11:07:16 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Nov 13 12:39:01 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Nov 13 17:49:25 EST 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -818,26 +834,26 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -854,10 +870,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -892,7 +908,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -944,7 +960,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1055,21 +1071,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1086,7 +1102,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1138,15 +1154,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
@@ -1154,18 +1170,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1205,10 +1221,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>239</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -1282,8 +1298,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1291,8 +1307,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
-  <dimension ref="A1:F41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -1300,13 +1316,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="16.28515625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2012,14 +2028,14 @@
   </sheetData>
   <autoFilter ref="A1:A41" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B11"/>
@@ -2027,9 +2043,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2377,14 +2393,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
-  <dimension ref="A1:M17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F11"/>
@@ -2392,20 +2408,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="28.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="38.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="21.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="21.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
+    <col min="14" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2449,7 +2465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -2470,7 +2486,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -2491,7 +2507,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -2511,7 +2527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -2531,7 +2547,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2551,7 +2567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -2571,7 +2587,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2591,7 +2607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2611,7 +2627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -2631,7 +2647,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2651,7 +2667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2671,7 +2687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2691,7 +2707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -2711,7 +2727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -2731,7 +2747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -2751,7 +2767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -2773,14 +2789,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -2788,18 +2804,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2890,13 +2906,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
@@ -2904,15 +2920,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -3109,13 +3125,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
-  <dimension ref="A1:L9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D9"/>
@@ -3123,19 +3139,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3279,7 +3295,7 @@
       <c r="I9" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3287,8 +3303,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
@@ -3296,11 +3312,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="3" max="4" style="1" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3359,8 +3375,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3368,8 +3384,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
@@ -3377,7 +3393,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="14.85546875" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3436,8 +3452,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3445,8 +3461,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -3454,19 +3470,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3544,7 +3560,7 @@
       <c r="I3" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3552,8 +3568,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -3561,13 +3577,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.140625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3642,8 +3658,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3651,8 +3667,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -3660,13 +3676,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3707,8 +3723,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3716,8 +3732,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
@@ -3725,15 +3741,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3967,8 +3983,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3976,8 +3992,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
-  <dimension ref="A1:L17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
@@ -3985,19 +4001,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="36" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="45.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="47.5703125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="36.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="35.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="45.5703125" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="47.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4472,13 +4488,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I13" r:id="rId1" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
-    <hyperlink ref="I12" r:id="rId2" xr:uid="{72B34BFC-1C06-4629-A7D1-00835E578F1C}"/>
-    <hyperlink ref="J12" r:id="rId3" xr:uid="{05843862-7C41-4D97-A198-1A33D27EECAF}"/>
-    <hyperlink ref="J13" r:id="rId4" xr:uid="{4B596713-18AE-4E73-886D-498F1C2E6C62}"/>
+    <hyperlink r:id="rId1" ref="I13" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
+    <hyperlink r:id="rId2" ref="I12" xr:uid="{72B34BFC-1C06-4629-A7D1-00835E578F1C}"/>
+    <hyperlink r:id="rId3" ref="J12" xr:uid="{05843862-7C41-4D97-A198-1A33D27EECAF}"/>
+    <hyperlink r:id="rId4" ref="J13" xr:uid="{4B596713-18AE-4E73-886D-498F1C2E6C62}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId5" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Made changes to RAD test cases and UM test cases.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{5FB401DB-C369-48E3-9BEA-1647B1D05DC1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E55B13D0-CD17-4563-B2FE-E732E6718FA9}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="13" firstSheet="10" windowHeight="14565" windowWidth="18810" xWindow="-20070" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="1185"/>
+    <workbookView activeTab="13" firstSheet="10" windowHeight="14565" windowWidth="18810" xWindow="4410" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="1665"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="244">
   <si>
     <t>Result</t>
   </si>
@@ -134,9 +134,6 @@
     <t>SearchType</t>
   </si>
   <si>
-    <t>chragui</t>
-  </si>
-  <si>
     <t>Exact Match</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>chra</t>
   </si>
   <si>
-    <t>agui</t>
-  </si>
-  <si>
     <t>hragu</t>
   </si>
   <si>
@@ -500,66 +494,12 @@
     <t>*Pp5</t>
   </si>
   <si>
-    <t>Sat Jul 01 21:39:01 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:39:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:40:02 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:40:32 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:41:03 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:41:32 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:42:00 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:42:28 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:42:56 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:43:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:43:53 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:44:22 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:44:50 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:45:18 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:45:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sat Jul 01 21:46:14 EDT 2023</t>
-  </si>
-  <si>
     <t>Hello@6666666</t>
   </si>
   <si>
     <t>hello2222</t>
   </si>
   <si>
-    <t>Wed Jul 05 20:23:01 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Jul 05 20:23:42 EDT 2023</t>
-  </si>
-  <si>
     <t>ToBeModUser</t>
   </si>
   <si>
@@ -584,45 +524,6 @@
     <t>Thu Jul 06 14:55:26 EDT 2023</t>
   </si>
   <si>
-    <t>Thu Jul 06 15:03:58 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 15:04:27 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 15:04:51 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 15:05:14 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 15:05:37 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 15:05:59 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 15:06:21 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 15:06:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 15:07:08 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 15:07:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 15:07:55 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 15:08:20 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 21:26:37 EDT 2023</t>
-  </si>
-  <si>
     <t>Tue Sep 19 21:27:07 EDT 2023</t>
   </si>
   <si>
@@ -737,9 +638,6 @@
     <t>Thu Sep 28 15:29:45 EDT 2023</t>
   </si>
   <si>
-    <t>Wed Nov 01 13:59:13 EDT 2023</t>
-  </si>
-  <si>
     <t>Wed Nov 01 13:59:42 EDT 2023</t>
   </si>
   <si>
@@ -758,19 +656,133 @@
     <t>Wed Nov 01 14:03:12 EDT 2023</t>
   </si>
   <si>
+    <t>Mon Nov 13 17:49:25 EST 2023</t>
+  </si>
+  <si>
+    <t>chraguis</t>
+  </si>
+  <si>
+    <t>aguis</t>
+  </si>
+  <si>
+    <t>Mon Dec 11 21:46:20 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Dec 11 21:46:49 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Dec 11 21:47:15 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Dec 11 21:47:39 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Dec 11 21:48:03 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Dec 11 21:48:26 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Dec 11 21:48:49 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Dec 11 21:49:13 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Dec 11 21:49:38 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Dec 11 21:50:01 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Dec 11 21:50:23 EST 2023</t>
+  </si>
+  <si>
+    <t>Mon Dec 11 21:50:47 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:23:40 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:24:12 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:24:42 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:25:09 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:25:38 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:26:08 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:26:38 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:27:06 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:27:33 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:27:59 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:28:29 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:28:58 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:29:26 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:29:55 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:30:26 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 12:30:55 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 13:06:04 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 13:17:41 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 13:18:23 EST 2023</t>
+  </si>
+  <si>
+    <t>Defect 7284</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Mon Nov 13 11:00:06 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Nov 13 11:07:16 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Nov 13 12:39:01 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Nov 13 17:49:25 EST 2023</t>
+    <t>Tue Dec 12 13:22:30 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 13:22:59 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 13:23:29 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 13:23:59 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 13:24:28 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 13:24:58 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 13:25:25 EST 2023</t>
   </si>
 </sst>
 </file>
@@ -1221,10 +1233,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
+        <v>201</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -1236,10 +1248,10 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
@@ -1247,10 +1259,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>157</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1262,10 +1274,10 @@
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
@@ -1273,10 +1285,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>158</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -1288,10 +1300,10 @@
         <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
@@ -1347,682 +1359,682 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F41" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2064,10 +2076,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -2075,10 +2087,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -2086,10 +2098,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -2097,10 +2109,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -2108,10 +2120,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -2119,10 +2131,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -2130,10 +2142,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -2141,10 +2153,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -2152,10 +2164,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -2163,10 +2175,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -2174,10 +2186,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -2185,10 +2197,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -2196,10 +2208,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -2207,10 +2219,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -2218,10 +2230,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -2229,10 +2241,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -2240,10 +2252,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -2251,10 +2263,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -2262,10 +2274,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -2273,10 +2285,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -2284,10 +2296,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -2295,10 +2307,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -2306,10 +2318,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -2317,10 +2329,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -2328,10 +2340,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -2339,10 +2351,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -2350,10 +2362,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -2361,10 +2373,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -2372,10 +2384,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -2383,10 +2395,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -2441,10 +2453,10 @@
         <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -2467,19 +2479,19 @@
     </row>
     <row ht="30" r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>216</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G2" s="3">
         <v>9</v>
@@ -2488,19 +2500,19 @@
     </row>
     <row ht="30" r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>217</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="G3" s="3">
         <v>9</v>
@@ -2509,19 +2521,19 @@
     </row>
     <row ht="30" r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>218</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G4" s="3">
         <v>9</v>
@@ -2529,19 +2541,19 @@
     </row>
     <row ht="30" r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>219</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G5" s="3">
         <v>9</v>
@@ -2549,19 +2561,19 @@
     </row>
     <row ht="30" r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>220</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G6" s="3">
         <v>9</v>
@@ -2569,19 +2581,19 @@
     </row>
     <row ht="30" r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>221</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G7" s="3">
         <v>9</v>
@@ -2589,19 +2601,19 @@
     </row>
     <row ht="30" r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>222</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G8" s="3">
         <v>9</v>
@@ -2609,19 +2621,19 @@
     </row>
     <row ht="30" r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G9" s="3">
         <v>9</v>
@@ -2629,19 +2641,19 @@
     </row>
     <row ht="30" r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>224</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G10" s="3">
         <v>10</v>
@@ -2649,19 +2661,19 @@
     </row>
     <row ht="30" r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>225</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
@@ -2669,19 +2681,19 @@
     </row>
     <row ht="30" r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>159</v>
+        <v>226</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G12" s="3">
         <v>10</v>
@@ -2689,19 +2701,19 @@
     </row>
     <row ht="30" r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G13" s="3">
         <v>10</v>
@@ -2709,19 +2721,19 @@
     </row>
     <row ht="30" r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G14" s="3">
         <v>10</v>
@@ -2729,19 +2741,19 @@
     </row>
     <row ht="30" r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>229</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G15" s="3">
         <v>10</v>
@@ -2749,19 +2761,19 @@
     </row>
     <row ht="30" r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>230</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G16" s="3">
         <v>10</v>
@@ -2769,19 +2781,19 @@
     </row>
     <row ht="30" r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>231</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G17" s="3">
         <v>10</v>
@@ -2855,10 +2867,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>233</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -2870,10 +2882,10 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
@@ -2881,10 +2893,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>234</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -2896,10 +2908,10 @@
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
@@ -2915,14 +2927,14 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="22.5703125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
@@ -2957,30 +2969,33 @@
         <v>26</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>237</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J2" s="3">
         <v>9</v>
@@ -2988,22 +3003,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J3" s="3">
         <v>9</v>
@@ -3011,22 +3026,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J4" s="3">
         <v>9</v>
@@ -3034,22 +3049,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J5" s="3">
         <v>9</v>
@@ -3057,22 +3072,22 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J6" s="3">
         <v>9</v>
@@ -3080,22 +3095,25 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>233</v>
+        <v>242</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J7" s="3">
         <v>9</v>
@@ -3103,22 +3121,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J8" s="3">
         <v>9</v>
@@ -3194,10 +3212,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3338,10 +3356,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3415,10 +3433,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3525,10 +3543,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3543,10 +3561,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3608,10 +3626,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3620,15 +3638,15 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3637,15 +3655,15 @@
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3654,7 +3672,7 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -3707,10 +3725,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3719,7 +3737,7 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3736,7 +3754,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3780,206 +3798,206 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>35</v>
+        <v>203</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>208</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>211</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>214</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -4051,429 +4069,429 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>177</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>178</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>179</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J4" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>180</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="J6" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>182</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>209</v>
+        <v>176</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>196</v>
+        <v>163</v>
       </c>
       <c r="J7" t="s">
-        <v>196</v>
+        <v>163</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>216</v>
+        <v>183</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>201</v>
+        <v>168</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>217</v>
+        <v>184</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>202</v>
+        <v>169</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>198</v>
+        <v>165</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>198</v>
+        <v>165</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>218</v>
+        <v>185</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>203</v>
+        <v>170</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>219</v>
+        <v>186</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>204</v>
+        <v>171</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>200</v>
+        <v>167</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>200</v>
+        <v>167</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>221</v>
+        <v>188</v>
       </c>
       <c r="E12" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>206</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>193</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>223</v>
+        <v>190</v>
       </c>
       <c r="F13" t="s">
-        <v>224</v>
+        <v>191</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>225</v>
+        <v>192</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>225</v>
+        <v>192</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>227</v>
+        <v>194</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>222</v>
+        <v>189</v>
       </c>
       <c r="F14" t="s">
-        <v>208</v>
+        <v>175</v>
       </c>
       <c r="G14" t="s">
-        <v>207</v>
+        <v>174</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>205</v>
+        <v>172</v>
       </c>
       <c r="J14" t="s">
-        <v>205</v>
+        <v>172</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added UM Role Test Cases and Data.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,39 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{E55B13D0-CD17-4563-B2FE-E732E6718FA9}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4091500F-069E-41A0-8049-E33B6E84F2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="13" firstSheet="10" windowHeight="14565" windowWidth="18810" xWindow="4410" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="1665"/>
+    <workbookView xWindow="2700" yWindow="1785" windowWidth="24525" windowHeight="14010" firstSheet="9" activeTab="15" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
-    <sheet name="CreateUserSpCharError" r:id="rId2" sheetId="2"/>
-    <sheet name="CreateUserSCFNameErr" r:id="rId3" sheetId="9"/>
-    <sheet name="CreateUserSCLNameErr" r:id="rId4" sheetId="10"/>
-    <sheet name="CreateUserSpChar" r:id="rId5" sheetId="3"/>
-    <sheet name="UsernameCase" r:id="rId6" sheetId="5"/>
-    <sheet name="PassCase" r:id="rId7" sheetId="6"/>
-    <sheet name="FindUser" r:id="rId8" sheetId="7"/>
-    <sheet name="CreateUserErrors" r:id="rId9" sheetId="8"/>
-    <sheet name="TestForTyler" r:id="rId10" sheetId="11"/>
-    <sheet name="TestLogin" r:id="rId11" sheetId="12"/>
-    <sheet name="CreateUserPasswordSpChar" r:id="rId12" sheetId="13"/>
-    <sheet name="ModifyUser" r:id="rId13" sheetId="14"/>
-    <sheet name="ModifyUserPwd" r:id="rId14" sheetId="15"/>
+    <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateUserSpCharError" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateUserSCFNameErr" sheetId="9" r:id="rId3"/>
+    <sheet name="CreateUserSCLNameErr" sheetId="10" r:id="rId4"/>
+    <sheet name="CreateUserSpChar" sheetId="3" r:id="rId5"/>
+    <sheet name="UsernameCase" sheetId="5" r:id="rId6"/>
+    <sheet name="PassCase" sheetId="6" r:id="rId7"/>
+    <sheet name="FindUser" sheetId="7" r:id="rId8"/>
+    <sheet name="CreateUserErrors" sheetId="8" r:id="rId9"/>
+    <sheet name="TestForTyler" sheetId="11" r:id="rId10"/>
+    <sheet name="TestLogin" sheetId="12" r:id="rId11"/>
+    <sheet name="CreateUserPasswordSpChar" sheetId="13" r:id="rId12"/>
+    <sheet name="ModifyUser" sheetId="14" r:id="rId13"/>
+    <sheet name="ModifyUserPwd" sheetId="15" r:id="rId14"/>
+    <sheet name="AddDeleteRole" sheetId="16" r:id="rId15"/>
+    <sheet name="SearchRole" sheetId="17" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">TestForTyler!$A$1:$A$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TestForTyler!$A$1:$A$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="249">
   <si>
     <t>Result</t>
   </si>
@@ -638,24 +640,6 @@
     <t>Thu Sep 28 15:29:45 EDT 2023</t>
   </si>
   <si>
-    <t>Wed Nov 01 13:59:42 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Nov 01 14:00:10 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Nov 01 14:00:38 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Nov 01 14:01:07 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Nov 01 14:02:47 EDT 2023</t>
-  </si>
-  <si>
-    <t>Wed Nov 01 14:03:12 EDT 2023</t>
-  </si>
-  <si>
     <t>Mon Nov 13 17:49:25 EST 2023</t>
   </si>
   <si>
@@ -749,9 +733,6 @@
     <t>Tue Dec 12 12:30:55 EST 2023</t>
   </si>
   <si>
-    <t>Tue Dec 12 13:06:04 EST 2023</t>
-  </si>
-  <si>
     <t>Tue Dec 12 13:17:41 EST 2023</t>
   </si>
   <si>
@@ -761,9 +742,6 @@
     <t>Defect 7284</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Tue Dec 12 13:22:30 EST 2023</t>
   </si>
   <si>
@@ -783,13 +761,51 @@
   </si>
   <si>
     <t>Tue Dec 12 13:25:25 EST 2023</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>JoinedRole</t>
+  </si>
+  <si>
+    <t>Dashes_in_Role</t>
+  </si>
+  <si>
+    <t>Space Role</t>
+  </si>
+  <si>
+    <t>NumberRole1</t>
+  </si>
+  <si>
+    <t>Fri Mar 22 18:49:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 22 18:49:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 22 18:50:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 22 18:50:39 EDT 2024</t>
+  </si>
+  <si>
+    <t>MelancholyKrat</t>
+  </si>
+  <si>
+    <t>Melancho</t>
+  </si>
+  <si>
+    <t>cholyKrat</t>
+  </si>
+  <si>
+    <t>lancho</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -846,26 +862,27 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -882,10 +899,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -920,7 +937,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -972,7 +989,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1083,21 +1100,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1114,7 +1131,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1166,34 +1183,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1236,7 +1253,7 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -1310,8 +1327,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1319,8 +1336,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
-  <dimension ref="A1:G41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -1328,13 +1345,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="16.28515625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="16.28515625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,14 +2057,14 @@
   </sheetData>
   <autoFilter ref="A1:A41" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B11"/>
@@ -2055,9 +2072,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2405,14 +2422,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
-  <dimension ref="A1:N17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F11"/>
@@ -2420,20 +2437,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="28.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="38.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="21.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="21.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
-    <col min="14" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2477,12 +2494,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>130</v>
@@ -2498,12 +2515,12 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row ht="30" r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>130</v>
@@ -2519,12 +2536,12 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row ht="30" r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>130</v>
@@ -2539,12 +2556,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>130</v>
@@ -2559,12 +2576,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>130</v>
@@ -2579,12 +2596,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>130</v>
@@ -2599,12 +2616,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>130</v>
@@ -2619,12 +2636,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>130</v>
@@ -2639,12 +2656,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>130</v>
@@ -2659,12 +2676,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>130</v>
@@ -2679,12 +2696,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>130</v>
@@ -2699,12 +2716,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>130</v>
@@ -2719,12 +2736,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>130</v>
@@ -2739,12 +2756,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>130</v>
@@ -2759,12 +2776,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>130</v>
@@ -2779,12 +2796,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>130</v>
@@ -2801,14 +2818,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -2816,18 +2833,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2870,7 +2887,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -2896,7 +2913,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -2918,29 +2935,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
-  <dimension ref="A1:K8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="22.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2980,10 +2997,10 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3006,7 +3023,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3029,7 +3046,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3052,7 +3069,7 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3075,7 +3092,7 @@
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -3098,10 +3115,10 @@
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -3124,7 +3141,7 @@
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -3143,13 +3160,211 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A53983D-C89C-4548-8A02-C36CB8EC5C28}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="5" collapsed="1"/>
+    <col min="5" max="5" width="18.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21" style="5" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABF931-E9E5-40BE-B844-C9FC3C47A38B}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="22.7109375" style="5" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="5"/>
+    <col min="5" max="5" width="24" style="5" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
-  <dimension ref="A1:M9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D9"/>
@@ -3157,19 +3372,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3313,7 +3528,7 @@
       <c r="I9" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3321,8 +3536,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
@@ -3330,11 +3545,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="4" style="1" width="9.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.140625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3393,8 +3608,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3402,8 +3617,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
@@ -3411,7 +3626,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="1" width="14.85546875" collapsed="true"/>
+    <col min="1" max="16384" width="14.85546875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3470,8 +3685,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3479,8 +3694,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -3488,19 +3703,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3578,7 +3793,7 @@
       <c r="I3" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3586,8 +3801,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -3595,13 +3810,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="22.140625" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3676,8 +3891,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3685,8 +3900,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -3694,13 +3909,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3741,8 +3956,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3750,8 +3965,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
@@ -3759,15 +3974,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3801,13 +4016,13 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>27</v>
@@ -3818,7 +4033,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3835,13 +4050,13 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>29</v>
@@ -3852,7 +4067,7 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3869,7 +4084,7 @@
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -3886,7 +4101,7 @@
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -3903,7 +4118,7 @@
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -3920,7 +4135,7 @@
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -3937,7 +4152,7 @@
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -3954,7 +4169,7 @@
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -3971,7 +4186,7 @@
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -3988,7 +4203,7 @@
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -4001,8 +4216,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4010,8 +4225,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
-  <dimension ref="A1:M17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
@@ -4019,19 +4234,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="36.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="35.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="45.5703125" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="47.5703125" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="36" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="35.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="45.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="47.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4506,13 +4721,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="I13" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
-    <hyperlink r:id="rId2" ref="I12" xr:uid="{72B34BFC-1C06-4629-A7D1-00835E578F1C}"/>
-    <hyperlink r:id="rId3" ref="J12" xr:uid="{05843862-7C41-4D97-A198-1A33D27EECAF}"/>
-    <hyperlink r:id="rId4" ref="J13" xr:uid="{4B596713-18AE-4E73-886D-498F1C2E6C62}"/>
+    <hyperlink ref="I13" r:id="rId1" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
+    <hyperlink ref="I12" r:id="rId2" xr:uid="{72B34BFC-1C06-4629-A7D1-00835E578F1C}"/>
+    <hyperlink ref="J12" r:id="rId3" xr:uid="{05843862-7C41-4D97-A198-1A33D27EECAF}"/>
+    <hyperlink ref="J13" r:id="rId4" xr:uid="{4B596713-18AE-4E73-886D-498F1C2E6C62}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId5" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updated IWP 2.3 Test Cases.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4091500F-069E-41A0-8049-E33B6E84F2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC67B92-4AE7-4AE3-813C-CA4C3235693C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="1785" windowWidth="24525" windowHeight="14010" firstSheet="9" activeTab="15" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="30270" yWindow="1005" windowWidth="24525" windowHeight="14010" firstSheet="10" activeTab="15" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="253">
   <si>
     <t>Result</t>
   </si>
@@ -800,6 +800,18 @@
   </si>
   <si>
     <t>lancho</t>
+  </si>
+  <si>
+    <t>Sat Mar 23 12:50:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Sat Mar 23 12:50:59 EDT 2024</t>
+  </si>
+  <si>
+    <t>Sat Mar 23 12:51:21 EDT 2024</t>
+  </si>
+  <si>
+    <t>Sat Mar 23 12:51:43 EDT 2024</t>
   </si>
 </sst>
 </file>
@@ -3169,7 +3181,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3285,12 +3297,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="22.7109375" style="5" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="5"/>
-    <col min="5" max="5" width="24" style="5" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.140625" style="5" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="5" collapsed="1"/>
+    <col min="5" max="5" width="24" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3314,6 +3326,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>249</v>
+      </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
@@ -3325,6 +3343,12 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>250</v>
+      </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
@@ -3336,6 +3360,12 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>251</v>
+      </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
@@ -3347,6 +3377,12 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>252</v>
+      </c>
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Updated button_Export and No ACH Debit Test Cases.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC67B92-4AE7-4AE3-813C-CA4C3235693C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9609CAA-8EF6-4EE9-B491-826BE81DD2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30270" yWindow="1005" windowWidth="24525" windowHeight="14010" firstSheet="10" activeTab="15" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="1877" yWindow="4509" windowWidth="14709" windowHeight="10182" activeTab="1" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="260">
   <si>
     <t>Result</t>
   </si>
@@ -505,9 +505,6 @@
     <t>ToBeModUser</t>
   </si>
   <si>
-    <t>Thu Jul 06 13:04:15 EDT 2023</t>
-  </si>
-  <si>
     <t>Thu Jul 06 13:18:47 EDT 2023</t>
   </si>
   <si>
@@ -812,6 +809,30 @@
   </si>
   <si>
     <t>Sat Mar 23 12:51:43 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon May 13 22:47:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon May 13 22:48:03 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon May 13 22:48:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon May 13 22:48:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon May 13 22:49:18 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon May 13 22:49:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon May 13 22:50:06 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon May 13 22:53:02 EDT 2024</t>
   </si>
 </sst>
 </file>
@@ -1209,23 +1230,23 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="14.15234375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.69140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.53515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.15234375" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.15234375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1260,12 +1281,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -1286,12 +1307,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1312,12 +1333,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -1355,18 +1376,18 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.3046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.15234375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="16.28515625" style="1" collapsed="1"/>
+    <col min="6" max="6" width="10.15234375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="16.3046875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1386,7 +1407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1403,7 +1424,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1420,7 +1441,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1437,7 +1458,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1454,7 +1475,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1471,7 +1492,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1488,7 +1509,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1505,7 +1526,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1522,7 +1543,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1539,7 +1560,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1556,7 +1577,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1573,7 +1594,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -1590,7 +1611,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1607,7 +1628,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1624,7 +1645,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1641,7 +1662,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1658,7 +1679,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -1675,7 +1696,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1692,7 +1713,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1709,7 +1730,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -1726,7 +1747,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1743,7 +1764,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1760,7 +1781,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -1777,7 +1798,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1794,7 +1815,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -1811,7 +1832,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1828,7 +1849,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1845,7 +1866,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1862,7 +1883,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -1879,7 +1900,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1896,7 +1917,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -1913,7 +1934,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -1930,7 +1951,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1947,7 +1968,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -1964,7 +1985,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -1981,7 +2002,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -1998,7 +2019,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -2015,7 +2036,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2032,7 +2053,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -2049,7 +2070,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -2082,14 +2103,14 @@
       <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.84375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.3046875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2103,7 +2124,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2114,7 +2135,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -2125,7 +2146,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -2136,7 +2157,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -2147,7 +2168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -2158,7 +2179,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -2169,7 +2190,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -2180,7 +2201,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2191,7 +2212,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -2202,7 +2223,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -2213,7 +2234,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2224,7 +2245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -2235,7 +2256,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2246,7 +2267,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -2257,7 +2278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2268,7 +2289,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2279,7 +2300,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -2290,7 +2311,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -2301,7 +2322,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2312,7 +2333,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -2323,7 +2344,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -2334,7 +2355,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2345,7 +2366,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2356,7 +2377,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -2367,7 +2388,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -2378,7 +2399,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2389,7 +2410,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2400,7 +2421,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2411,7 +2432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -2422,7 +2443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -2447,25 +2468,25 @@
       <selection activeCell="F2" sqref="F2:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="28" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.3046875" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="21" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.3046875" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.69140625" style="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="12" max="12" width="16.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.69140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="9.15234375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2506,12 +2527,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>130</v>
@@ -2527,12 +2548,12 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>130</v>
@@ -2548,12 +2569,12 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>130</v>
@@ -2568,12 +2589,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>130</v>
@@ -2588,12 +2609,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>130</v>
@@ -2608,12 +2629,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>130</v>
@@ -2628,12 +2649,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>130</v>
@@ -2648,12 +2669,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>130</v>
@@ -2668,12 +2689,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>130</v>
@@ -2688,12 +2709,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>130</v>
@@ -2708,12 +2729,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>130</v>
@@ -2728,12 +2749,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>130</v>
@@ -2748,12 +2769,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>130</v>
@@ -2768,12 +2789,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>130</v>
@@ -2788,12 +2809,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>130</v>
@@ -2808,12 +2829,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>130</v>
@@ -2843,23 +2864,23 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="14.15234375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.69140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.53515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.15234375" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.15234375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2894,12 +2915,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -2920,12 +2941,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -2959,20 +2980,20 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="19.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.3828125" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
+    <col min="5" max="5" width="22.53515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.84375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.69140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="19.3828125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3004,15 +3025,15 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3030,12 +3051,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3053,12 +3074,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3076,12 +3097,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3099,12 +3120,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -3122,15 +3143,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -3148,12 +3169,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -3184,17 +3205,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.140625" style="5" collapsed="1"/>
-    <col min="5" max="5" width="18.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="6.53515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.84375" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.15234375" style="5" collapsed="1"/>
+    <col min="5" max="5" width="18.3828125" style="5" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="21" style="5" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="7" max="16384" width="9.15234375" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3208,75 +3229,75 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>27</v>
@@ -3291,21 +3312,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABF931-E9E5-40BE-B844-C9FC3C47A38B}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" width="9.15234375" style="5" collapsed="1"/>
+    <col min="2" max="2" width="22.69140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.15234375" style="5" collapsed="1"/>
     <col min="5" max="5" width="24" style="5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="6" max="6" width="22.69140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.15234375" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3319,75 +3340,75 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>30</v>
@@ -3402,28 +3423,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.84375" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.15234375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.69140625" style="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="11" max="11" width="16.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.15234375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3461,12 +3482,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>252</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3479,7 +3500,13 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>253</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3491,7 +3518,13 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3503,7 +3536,13 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>255</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3515,7 +3554,13 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>256</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3527,7 +3572,13 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>257</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3539,7 +3590,13 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>258</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
@@ -3551,7 +3608,13 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>259</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
@@ -3579,16 +3642,16 @@
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" width="9.15234375" style="1" collapsed="1"/>
+    <col min="2" max="2" width="25.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.15234375" style="1" collapsed="1"/>
+    <col min="5" max="5" width="12.15234375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.15234375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3605,12 +3668,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3619,7 +3682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3627,7 +3690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3635,7 +3698,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3660,12 +3723,12 @@
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="14.85546875" style="1" collapsed="1"/>
+    <col min="1" max="16384" width="14.84375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3682,12 +3745,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3696,7 +3759,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3704,7 +3767,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3712,7 +3775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3737,24 +3800,24 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.84375" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.15234375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.69140625" style="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="11" max="11" width="16.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.15234375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3792,12 +3855,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3810,12 +3873,12 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3844,18 +3907,18 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="6" max="6" width="22.15234375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.15234375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3875,12 +3938,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3892,12 +3955,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3909,12 +3972,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3943,18 +4006,18 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="6" max="6" width="14.84375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.15234375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3974,12 +4037,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -4008,20 +4071,20 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="19.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
+    <col min="6" max="6" width="13.84375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.69140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="19.3828125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4047,29 +4110,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -4081,29 +4144,29 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -4115,12 +4178,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -4132,12 +4195,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -4149,12 +4212,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -4166,12 +4229,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -4183,12 +4246,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -4200,12 +4263,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -4217,12 +4280,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -4234,12 +4297,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -4268,24 +4331,24 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="47.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.3046875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.84375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.53515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="36" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="45.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="47.5703125" style="1" collapsed="1"/>
+    <col min="10" max="10" width="35.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="45.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="47.53515625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4323,12 +4386,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>48</v>
@@ -4355,12 +4418,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>48</v>
@@ -4387,12 +4450,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>48</v>
@@ -4419,12 +4482,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>23</v>
@@ -4451,15 +4514,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>46</v>
@@ -4480,18 +4543,18 @@
         <v>14</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>46</v>
@@ -4503,27 +4566,27 @@
         <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>46</v>
@@ -4535,27 +4598,27 @@
         <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>46</v>
@@ -4567,27 +4630,27 @@
         <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>46</v>
@@ -4599,27 +4662,27 @@
         <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>46</v>
@@ -4631,27 +4694,27 @@
         <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>46</v>
@@ -4663,33 +4726,33 @@
         <v>13</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F13" t="s">
         <v>190</v>
-      </c>
-      <c r="F13" t="s">
-        <v>191</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>47</v>
@@ -4698,60 +4761,60 @@
         <v>13</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B16"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Test Data for Create User.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,41 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9609CAA-8EF6-4EE9-B491-826BE81DD2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{2E5C556C-D189-4A9B-AA40-A81EF7903069}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="1877" yWindow="4509" windowWidth="14709" windowHeight="10182" activeTab="1" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView activeTab="1" windowHeight="21220" windowWidth="38620" xWindow="-38510" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-2030"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
-    <sheet name="CreateUserSpCharError" sheetId="2" r:id="rId2"/>
-    <sheet name="CreateUserSCFNameErr" sheetId="9" r:id="rId3"/>
-    <sheet name="CreateUserSCLNameErr" sheetId="10" r:id="rId4"/>
-    <sheet name="CreateUserSpChar" sheetId="3" r:id="rId5"/>
-    <sheet name="UsernameCase" sheetId="5" r:id="rId6"/>
-    <sheet name="PassCase" sheetId="6" r:id="rId7"/>
-    <sheet name="FindUser" sheetId="7" r:id="rId8"/>
-    <sheet name="CreateUserErrors" sheetId="8" r:id="rId9"/>
-    <sheet name="TestForTyler" sheetId="11" r:id="rId10"/>
-    <sheet name="TestLogin" sheetId="12" r:id="rId11"/>
-    <sheet name="CreateUserPasswordSpChar" sheetId="13" r:id="rId12"/>
-    <sheet name="ModifyUser" sheetId="14" r:id="rId13"/>
-    <sheet name="ModifyUserPwd" sheetId="15" r:id="rId14"/>
-    <sheet name="AddDeleteRole" sheetId="16" r:id="rId15"/>
-    <sheet name="SearchRole" sheetId="17" r:id="rId16"/>
+    <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
+    <sheet name="CreateUserSpCharError" r:id="rId2" sheetId="2"/>
+    <sheet name="CreateUserSCFNameErr" r:id="rId3" sheetId="9"/>
+    <sheet name="CreateUserSCLNameErr" r:id="rId4" sheetId="10"/>
+    <sheet name="CreateUserSpChar" r:id="rId5" sheetId="3"/>
+    <sheet name="UsernameCase" r:id="rId6" sheetId="5"/>
+    <sheet name="PassCase" r:id="rId7" sheetId="6"/>
+    <sheet name="FindUser" r:id="rId8" sheetId="7"/>
+    <sheet name="CreateUserErrors" r:id="rId9" sheetId="8"/>
+    <sheet name="TestForTyler" r:id="rId10" sheetId="11"/>
+    <sheet name="TestLogin" r:id="rId11" sheetId="12"/>
+    <sheet name="CreateUserPasswordSpChar" r:id="rId12" sheetId="13"/>
+    <sheet name="ModifyUser" r:id="rId13" sheetId="14"/>
+    <sheet name="ModifyUserPwd" r:id="rId14" sheetId="15"/>
+    <sheet name="AddDeleteRole" r:id="rId15" sheetId="16"/>
+    <sheet name="SearchRole" r:id="rId16" sheetId="17"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TestForTyler!$A$1:$A$41</definedName>
+    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">TestForTyler!$A$1:$A$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="262">
   <si>
     <t>Result</t>
   </si>
@@ -811,34 +811,41 @@
     <t>Sat Mar 23 12:51:43 EDT 2024</t>
   </si>
   <si>
-    <t>Mon May 13 22:47:35 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon May 13 22:48:03 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon May 13 22:48:26 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon May 13 22:48:50 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon May 13 22:49:18 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon May 13 22:49:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon May 13 22:50:06 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon May 13 22:53:02 EDT 2024</t>
+    <t>Tue May 14 14:17:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue May 14 14:18:23 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue May 14 14:18:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue May 14 14:19:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue May 14 14:20:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue May 14 14:20:31 EDT 2024</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Tue May 14 14:35:45 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue May 14 14:36:21 EDT 2024</t>
+  </si>
+  <si>
+    <t>Tue May 14 14:36:56 EDT 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -895,27 +902,27 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -932,10 +939,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -970,7 +977,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1022,7 +1029,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1133,21 +1140,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1164,7 +1171,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1216,15 +1223,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -1232,18 +1239,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.15234375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.69140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.53515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.15234375" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.15234375" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="14.15234375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.84375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.3828125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="23.53515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="29.15234375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.84375" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.15234375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
@@ -1360,8 +1367,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1369,8 +1376,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
-  <dimension ref="A1:F41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -1378,13 +1385,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.15234375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.15234375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="16.3046875" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.15234375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="10.15234375" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="16.3046875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
@@ -2090,14 +2097,14 @@
   </sheetData>
   <autoFilter ref="A1:A41" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B11"/>
@@ -2105,9 +2112,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="34.84375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.3046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="34.84375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.3046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
@@ -2455,14 +2462,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
-  <dimension ref="A1:M17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F11"/>
@@ -2470,20 +2477,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.3046875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.3046875" style="3" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.69140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.69140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="9.15234375" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="28.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="38.3046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="21.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="21.3046875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.84375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.3828125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="16.69140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="12.69140625" collapsed="true"/>
+    <col min="14" max="16384" style="1" width="9.15234375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
@@ -2527,7 +2534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2548,7 +2555,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -2569,7 +2576,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -2589,7 +2596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -2609,7 +2616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -2629,7 +2636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -2649,7 +2656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -2669,7 +2676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2689,7 +2696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -2709,7 +2716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -2729,7 +2736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2749,7 +2756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -2769,7 +2776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2789,7 +2796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -2809,7 +2816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2829,7 +2836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
+    <row ht="29.15" r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2851,14 +2858,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -2866,18 +2873,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.15234375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.69140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.53515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="29.15234375" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.15234375" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="14.15234375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.84375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.3828125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="23.53515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="29.15234375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.84375" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.15234375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
@@ -2968,13 +2975,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -2982,15 +2989,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.3828125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.53515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.84375" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.69140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="19.3828125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.3828125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.53515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.84375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.69140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.3828125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="19.3828125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
@@ -3193,13 +3200,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A53983D-C89C-4548-8A02-C36CB8EC5C28}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A53983D-C89C-4548-8A02-C36CB8EC5C28}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -3207,12 +3214,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.53515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.84375" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.15234375" style="5" collapsed="1"/>
-    <col min="5" max="5" width="18.3828125" style="5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21" style="5" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.15234375" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="6.53515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="29.84375" collapsed="true"/>
+    <col min="3" max="4" style="5" width="9.15234375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="18.3828125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="21.0" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.15234375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
@@ -3304,12 +3311,302 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABF931-E9E5-40BE-B844-C9FC3C47A38B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABF931-E9E5-40BE-B844-C9FC3C47A38B}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" style="5" width="9.15234375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="22.69140625" collapsed="true"/>
+    <col min="3" max="4" style="5" width="9.15234375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="24.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="22.69140625" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.15234375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.84375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.15234375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.84375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.3828125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.69140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.84375" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.15234375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>257</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3318,337 +3615,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.15234375" style="5" collapsed="1"/>
-    <col min="2" max="2" width="22.69140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.15234375" style="5" collapsed="1"/>
-    <col min="5" max="5" width="24" style="5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.69140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.15234375" style="5" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>248</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>249</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>250</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>251</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
-  <dimension ref="A1:L9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.84375" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.15234375" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="26.69140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="4.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="9.15234375" style="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>253</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>254</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>255</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" t="s">
-        <v>256</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>257</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>259</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="9.15234375" style="1" collapsed="1"/>
-    <col min="2" max="2" width="25.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.15234375" style="1" collapsed="1"/>
-    <col min="5" max="5" width="12.15234375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.15234375" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.15234375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.84375" collapsed="true"/>
+    <col min="3" max="4" style="1" width="9.15234375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.15234375" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.15234375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
@@ -3707,8 +3678,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3716,8 +3687,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
@@ -3725,7 +3696,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="14.84375" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="14.84375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
@@ -3784,8 +3755,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3793,28 +3764,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.84375" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.15234375" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="26.69140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="4.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="9.15234375" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.84375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.84375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.15234375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.84375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.3828125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.69140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.84375" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.15234375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
@@ -3860,7 +3831,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>259</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3878,7 +3849,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>260</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3891,8 +3862,25 @@
       </c>
       <c r="I3" s="2"/>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3900,8 +3888,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -3909,13 +3897,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.15234375" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.15234375" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.84375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.15234375" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.15234375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
@@ -3990,8 +3978,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3999,8 +3987,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -4008,13 +3996,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.84375" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.15234375" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.84375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.84375" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.15234375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
@@ -4055,8 +4043,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4064,8 +4052,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
@@ -4073,15 +4061,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.84375" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.69140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="19.3828125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.84375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.84375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.69140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.3828125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="19.3828125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
@@ -4315,8 +4303,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4324,8 +4312,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
-  <dimension ref="A1:L17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
@@ -4333,19 +4321,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.69140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.3046875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.84375" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.53515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="36" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="35.3828125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.84375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="45.53515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16384" width="47.53515625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="18.3046875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="19.84375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="20.53515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="23.84375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="36.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="35.3828125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.84375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="45.53515625" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="47.53515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
@@ -4820,13 +4808,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I13" r:id="rId1" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
-    <hyperlink ref="I12" r:id="rId2" xr:uid="{72B34BFC-1C06-4629-A7D1-00835E578F1C}"/>
-    <hyperlink ref="J12" r:id="rId3" xr:uid="{05843862-7C41-4D97-A198-1A33D27EECAF}"/>
-    <hyperlink ref="J13" r:id="rId4" xr:uid="{4B596713-18AE-4E73-886D-498F1C2E6C62}"/>
+    <hyperlink r:id="rId1" ref="I13" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
+    <hyperlink r:id="rId2" ref="I12" xr:uid="{72B34BFC-1C06-4629-A7D1-00835E578F1C}"/>
+    <hyperlink r:id="rId3" ref="J12" xr:uid="{05843862-7C41-4D97-A198-1A33D27EECAF}"/>
+    <hyperlink r:id="rId4" ref="J13" xr:uid="{4B596713-18AE-4E73-886D-498F1C2E6C62}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId5" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Added VT-SuccessfulPayment-CC Test case and keywords for comparison with UiPath.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="336">
   <si>
     <t>Result</t>
   </si>
@@ -848,6 +848,219 @@
   </si>
   <si>
     <t>Mon Jun 03 17:41:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:51:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:52:20 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:52:52 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:53:24 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:53:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:54:25 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:54:56 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:55:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:55:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:56:04 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:56:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:56:50 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:57:13 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:57:43 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:58:09 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:58:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:59:03 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:59:27 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 18:59:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:00:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:00:46 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:01:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:01:39 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:02:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:02:31 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:02:40 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:02:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:03:10 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:03:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:03:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:04:25 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:04:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:05:24 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:05:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:06:24 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:06:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:07:24 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:07:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:08:23 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:08:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:09:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:09:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:10:22 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:10:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:12:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:13:21 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:13:53 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:14:25 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:14:57 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:15:28 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:15:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:16:28 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:17:08 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:17:49 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:18:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:18:36 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:18:58 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:19:21 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:19:45 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:20:07 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:20:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:20:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:21:16 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:22:46 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:23:14 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:23:40 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:24:06 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:24:32 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:24:57 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:25:19 EDT 2024</t>
+  </si>
+  <si>
+    <t>Fri Jul 12 19:25:41 EDT 2024</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1515,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -1328,7 +1541,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1354,7 +1567,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -2548,7 +2761,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>293</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>130</v>
@@ -2569,7 +2782,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>294</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>130</v>
@@ -2590,7 +2803,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>295</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>130</v>
@@ -2610,7 +2823,7 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>296</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>130</v>
@@ -2630,7 +2843,7 @@
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>297</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>130</v>
@@ -2650,7 +2863,7 @@
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>214</v>
+        <v>298</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>130</v>
@@ -2670,7 +2883,7 @@
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>215</v>
+        <v>299</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>130</v>
@@ -2690,7 +2903,7 @@
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>216</v>
+        <v>300</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>130</v>
@@ -2710,7 +2923,7 @@
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>217</v>
+        <v>301</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>130</v>
@@ -2730,7 +2943,7 @@
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>218</v>
+        <v>302</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>130</v>
@@ -2750,7 +2963,7 @@
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>219</v>
+        <v>303</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>130</v>
@@ -2770,7 +2983,7 @@
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>220</v>
+        <v>304</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>130</v>
@@ -2790,7 +3003,7 @@
         <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>221</v>
+        <v>305</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>130</v>
@@ -2810,7 +3023,7 @@
         <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>306</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>130</v>
@@ -2830,7 +3043,7 @@
         <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>223</v>
+        <v>307</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>130</v>
@@ -2850,7 +3063,7 @@
         <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>224</v>
+        <v>308</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>130</v>
@@ -2936,7 +3149,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>225</v>
+        <v>316</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -2962,7 +3175,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>226</v>
+        <v>317</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3046,7 +3259,7 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>309</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>227</v>
@@ -3072,7 +3285,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>310</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3095,7 +3308,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>230</v>
+        <v>311</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3118,7 +3331,7 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>231</v>
+        <v>312</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3141,7 +3354,7 @@
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>232</v>
+        <v>313</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -3164,7 +3377,7 @@
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>233</v>
+        <v>314</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>227</v>
@@ -3190,7 +3403,7 @@
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>234</v>
+        <v>315</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -3256,7 +3469,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>328</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -3273,7 +3486,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>241</v>
+        <v>329</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
@@ -3290,7 +3503,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>330</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
@@ -3307,7 +3520,7 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>331</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>11</v>
@@ -3367,7 +3580,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>248</v>
+        <v>332</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -3384,7 +3597,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>333</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
@@ -3401,7 +3614,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
@@ -3418,7 +3631,7 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>251</v>
+        <v>335</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>11</v>
@@ -3503,7 +3716,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3521,7 +3734,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3539,7 +3752,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3557,7 +3770,7 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>274</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3575,7 +3788,7 @@
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -3593,7 +3806,7 @@
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -3653,7 +3866,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>318</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3663,6 +3876,12 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>319</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3671,6 +3890,12 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>320</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3679,6 +3904,12 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>321</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3730,7 +3961,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>322</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3740,6 +3971,12 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>323</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3748,6 +3985,12 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>324</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3756,6 +3999,12 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>325</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3840,7 +4089,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3858,7 +4107,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3876,7 +4125,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3940,7 +4189,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>290</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3957,7 +4206,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>291</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3974,7 +4223,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>292</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -4039,7 +4288,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>289</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -4112,7 +4361,7 @@
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>277</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -4129,7 +4378,7 @@
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>278</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -4146,7 +4395,7 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>279</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -4163,7 +4412,7 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -4180,7 +4429,7 @@
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>281</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -4197,7 +4446,7 @@
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>282</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -4214,7 +4463,7 @@
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>203</v>
+        <v>283</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -4231,7 +4480,7 @@
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>284</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -4248,7 +4497,7 @@
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -4265,7 +4514,7 @@
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>206</v>
+        <v>286</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -4282,7 +4531,7 @@
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>287</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -4299,7 +4548,7 @@
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>288</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -4740,7 +4989,7 @@
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>192</v>
+        <v>326</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -4775,7 +5024,7 @@
         <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>193</v>
+        <v>327</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Updated CreditThem for Marina and added initial BDD files
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,41 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{2E5C556C-D189-4A9B-AA40-A81EF7903069}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F360F8C9-925E-4E3C-8B12-D64FEE1658F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="21220" windowWidth="38620" xWindow="-38510" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-2030"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
-    <sheet name="CreateUserSpCharError" r:id="rId2" sheetId="2"/>
-    <sheet name="CreateUserSCFNameErr" r:id="rId3" sheetId="9"/>
-    <sheet name="CreateUserSCLNameErr" r:id="rId4" sheetId="10"/>
-    <sheet name="CreateUserSpChar" r:id="rId5" sheetId="3"/>
-    <sheet name="UsernameCase" r:id="rId6" sheetId="5"/>
-    <sheet name="PassCase" r:id="rId7" sheetId="6"/>
-    <sheet name="FindUser" r:id="rId8" sheetId="7"/>
-    <sheet name="CreateUserErrors" r:id="rId9" sheetId="8"/>
-    <sheet name="TestForTyler" r:id="rId10" sheetId="11"/>
-    <sheet name="TestLogin" r:id="rId11" sheetId="12"/>
-    <sheet name="CreateUserPasswordSpChar" r:id="rId12" sheetId="13"/>
-    <sheet name="ModifyUser" r:id="rId13" sheetId="14"/>
-    <sheet name="ModifyUserPwd" r:id="rId14" sheetId="15"/>
-    <sheet name="AddDeleteRole" r:id="rId15" sheetId="16"/>
-    <sheet name="SearchRole" r:id="rId16" sheetId="17"/>
+    <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateUserSpCharError" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateUserSCFNameErr" sheetId="9" r:id="rId3"/>
+    <sheet name="CreateUserSCLNameErr" sheetId="10" r:id="rId4"/>
+    <sheet name="CreateUserSpChar" sheetId="3" r:id="rId5"/>
+    <sheet name="UsernameCase" sheetId="5" r:id="rId6"/>
+    <sheet name="PassCase" sheetId="6" r:id="rId7"/>
+    <sheet name="FindUser" sheetId="7" r:id="rId8"/>
+    <sheet name="CreateUserErrors" sheetId="8" r:id="rId9"/>
+    <sheet name="TestForTyler" sheetId="11" r:id="rId10"/>
+    <sheet name="TestLogin" sheetId="12" r:id="rId11"/>
+    <sheet name="CreateUserPasswordSpChar" sheetId="13" r:id="rId12"/>
+    <sheet name="ModifyUser" sheetId="14" r:id="rId13"/>
+    <sheet name="ModifyUserPwd" sheetId="15" r:id="rId14"/>
+    <sheet name="AddDeleteRole" sheetId="16" r:id="rId15"/>
+    <sheet name="SearchRole" sheetId="17" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">TestForTyler!$A$1:$A$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">TestForTyler!$A$1:$A$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="265">
   <si>
     <t>Result</t>
   </si>
@@ -505,36 +505,6 @@
     <t>ToBeModUser</t>
   </si>
   <si>
-    <t>Thu Jul 06 13:18:47 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 13:27:01 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 14:40:53 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 14:41:11 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 14:41:25 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Jul 06 14:55:26 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 21:27:07 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 21:27:34 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 21:30:10 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Sep 19 21:30:40 EDT 2023</t>
-  </si>
-  <si>
     <t>username236</t>
   </si>
   <si>
@@ -631,135 +601,15 @@
     <t>Gorbachovaaaab@1</t>
   </si>
   <si>
-    <t>Thu Sep 28 15:29:18 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Sep 28 15:29:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Nov 13 17:49:25 EST 2023</t>
-  </si>
-  <si>
     <t>chraguis</t>
   </si>
   <si>
     <t>aguis</t>
   </si>
   <si>
-    <t>Mon Dec 11 21:46:20 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:46:49 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:47:15 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:47:39 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:48:03 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:48:26 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:48:49 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:49:13 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:49:38 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:50:01 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:50:23 EST 2023</t>
-  </si>
-  <si>
-    <t>Mon Dec 11 21:50:47 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:23:40 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:24:12 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:24:42 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:25:09 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:25:38 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:26:08 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:26:38 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:27:06 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:27:33 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:27:59 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:28:29 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:28:58 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:29:26 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:29:55 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:30:26 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 12:30:55 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 13:17:41 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 13:18:23 EST 2023</t>
-  </si>
-  <si>
     <t>Defect 7284</t>
   </si>
   <si>
-    <t>Tue Dec 12 13:22:30 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 13:22:59 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 13:23:29 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 13:23:59 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 13:24:28 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 13:24:58 EST 2023</t>
-  </si>
-  <si>
-    <t>Tue Dec 12 13:25:25 EST 2023</t>
-  </si>
-  <si>
     <t>RoleName</t>
   </si>
   <si>
@@ -775,18 +625,6 @@
     <t>NumberRole1</t>
   </si>
   <si>
-    <t>Fri Mar 22 18:49:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 22 18:49:49 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 22 18:50:15 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Mar 22 18:50:39 EDT 2024</t>
-  </si>
-  <si>
     <t>MelancholyKrat</t>
   </si>
   <si>
@@ -797,57 +635,6 @@
   </si>
   <si>
     <t>lancho</t>
-  </si>
-  <si>
-    <t>Sat Mar 23 12:50:34 EDT 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 23 12:50:59 EDT 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 23 12:51:21 EDT 2024</t>
-  </si>
-  <si>
-    <t>Sat Mar 23 12:51:43 EDT 2024</t>
-  </si>
-  <si>
-    <t>Tue May 14 14:17:55 EDT 2024</t>
-  </si>
-  <si>
-    <t>Tue May 14 14:18:23 EDT 2024</t>
-  </si>
-  <si>
-    <t>Tue May 14 14:18:48 EDT 2024</t>
-  </si>
-  <si>
-    <t>Tue May 14 14:19:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Tue May 14 14:20:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Tue May 14 14:20:31 EDT 2024</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Tue May 14 14:35:45 EDT 2024</t>
-  </si>
-  <si>
-    <t>Tue May 14 14:36:21 EDT 2024</t>
-  </si>
-  <si>
-    <t>Tue May 14 14:36:56 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Jun 03 17:40:18 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Jun 03 17:40:55 EDT 2024</t>
-  </si>
-  <si>
-    <t>Mon Jun 03 17:41:29 EDT 2024</t>
   </si>
   <si>
     <t>Fri Jul 12 18:51:44 EDT 2024</t>
@@ -1067,7 +854,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1124,27 +910,27 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1157,14 +943,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1197,9 +983,9 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1251,7 +1037,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1303,7 +1089,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1362,21 +1148,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1393,7 +1179,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1445,37 +1231,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="14.15234375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.84375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.3828125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.53515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="29.15234375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.84375" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.15234375" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1510,12 +1296,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>265</v>
+        <v>194</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -1536,12 +1322,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>266</v>
+        <v>195</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1562,12 +1348,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>267</v>
+        <v>196</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -1589,8 +1375,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1598,25 +1384,25 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
-  <dimension ref="A1:G41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}">
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.15234375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="10.15234375" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="16.3046875" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="16.28515625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1636,7 +1422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1653,7 +1439,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1670,7 +1456,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1687,7 +1473,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1704,7 +1490,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1721,7 +1507,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1738,7 +1524,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1755,7 +1541,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1772,7 +1558,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1789,7 +1575,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1806,7 +1592,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1823,7 +1609,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -1840,7 +1626,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1857,7 +1643,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1874,7 +1660,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1891,7 +1677,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1908,7 +1694,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -1925,7 +1711,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1942,7 +1728,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1959,7 +1745,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -1976,7 +1762,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1993,7 +1779,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2010,7 +1796,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2027,7 +1813,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -2044,7 +1830,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -2061,7 +1847,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2078,7 +1864,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2095,7 +1881,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2112,7 +1898,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -2129,7 +1915,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -2146,7 +1932,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -2163,7 +1949,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -2180,7 +1966,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -2197,7 +1983,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -2214,7 +2000,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -2231,7 +2017,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -2248,7 +2034,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -2265,7 +2051,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2282,7 +2068,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -2299,7 +2085,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -2319,27 +2105,27 @@
   </sheetData>
   <autoFilter ref="A1:A41" xr:uid="{06D08B5C-751A-493E-80A1-F414BB27DBFB}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448B252B-DA85-45B5-97C8-A61A3A927843}">
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="34.84375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.3046875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2353,7 +2139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2364,7 +2150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -2375,7 +2161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -2386,7 +2172,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -2397,7 +2183,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -2408,7 +2194,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -2419,7 +2205,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -2430,7 +2216,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2441,7 +2227,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -2452,7 +2238,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -2463,7 +2249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2474,7 +2260,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -2485,7 +2271,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2496,7 +2282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -2507,7 +2293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2518,7 +2304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2529,7 +2315,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -2540,7 +2326,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -2551,7 +2337,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2562,7 +2348,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -2573,7 +2359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -2584,7 +2370,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2595,7 +2381,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2606,7 +2392,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -2617,7 +2403,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -2628,7 +2414,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2639,7 +2425,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2650,7 +2436,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2661,7 +2447,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -2672,7 +2458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -2684,38 +2470,38 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
-  <dimension ref="A1:N17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="28.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="38.3046875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="21.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="21.3046875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.84375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.3828125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="16.69140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="12.69140625" collapsed="true"/>
-    <col min="14" max="16384" style="1" width="9.15234375" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2756,12 +2542,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="29.15" r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>222</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>130</v>
@@ -2777,12 +2563,12 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row ht="29.15" r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>223</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>130</v>
@@ -2798,12 +2584,12 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row ht="29.15" r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>295</v>
+        <v>224</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>130</v>
@@ -2818,12 +2604,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="29.15" r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>296</v>
+        <v>225</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>130</v>
@@ -2838,12 +2624,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="29.15" r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>297</v>
+        <v>226</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>130</v>
@@ -2858,12 +2644,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="29.15" r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>298</v>
+        <v>227</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>130</v>
@@ -2878,12 +2664,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="29.15" r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>299</v>
+        <v>228</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>130</v>
@@ -2898,12 +2684,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="29.15" r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>300</v>
+        <v>229</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>130</v>
@@ -2918,12 +2704,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="29.15" r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>301</v>
+        <v>230</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>130</v>
@@ -2938,12 +2724,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="29.15" r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>302</v>
+        <v>231</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>130</v>
@@ -2958,12 +2744,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="29.15" r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>303</v>
+        <v>232</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>130</v>
@@ -2978,12 +2764,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="29.15" r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>304</v>
+        <v>233</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>130</v>
@@ -2998,12 +2784,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="29.15" r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>305</v>
+        <v>234</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>130</v>
@@ -3018,12 +2804,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="29.15" r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>306</v>
+        <v>235</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>130</v>
@@ -3038,12 +2824,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="29.15" r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>307</v>
+        <v>236</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>130</v>
@@ -3058,12 +2844,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="29.15" r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>308</v>
+        <v>237</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>130</v>
@@ -3080,36 +2866,36 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B8F5FA-1070-472D-B967-69AFD2883CDC}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="14.15234375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.84375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.3828125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.53515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="29.15234375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.84375" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.15234375" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="29.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3144,12 +2930,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>316</v>
+        <v>245</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3170,12 +2956,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>317</v>
+        <v>246</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3197,32 +2983,32 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
-  <dimension ref="A1:K8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A7FE5-E252-4628-A48A-457CABF49F07}">
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.3828125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="22.53515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="13.84375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.69140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.3828125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="19.3828125" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3254,15 +3040,15 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>309</v>
+        <v>238</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>227</v>
+        <v>184</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3280,12 +3066,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>310</v>
+        <v>239</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3303,12 +3089,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>311</v>
+        <v>240</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3326,12 +3112,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>312</v>
+        <v>241</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3349,12 +3135,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>313</v>
+        <v>242</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -3372,15 +3158,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>314</v>
+        <v>243</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>227</v>
+        <v>184</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -3398,12 +3184,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>315</v>
+        <v>244</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -3422,29 +3208,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A53983D-C89C-4548-8A02-C36CB8EC5C28}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A53983D-C89C-4548-8A02-C36CB8EC5C28}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="29.84375" collapsed="true"/>
-    <col min="3" max="4" style="5" width="9.15234375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="18.3828125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="5" width="21.0" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.15234375" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="5" collapsed="1"/>
+    <col min="5" max="5" width="18.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21" style="5" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3458,104 +3244,104 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>328</v>
+        <v>257</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>238</v>
+        <v>188</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>258</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>330</v>
+        <v>259</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>237</v>
+        <v>187</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>331</v>
+        <v>260</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>239</v>
+        <v>189</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABF931-E9E5-40BE-B844-C9FC3C47A38B}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABF931-E9E5-40BE-B844-C9FC3C47A38B}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.15234375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="22.69140625" collapsed="true"/>
-    <col min="3" max="4" style="5" width="9.15234375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="24.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="5" width="22.69140625" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.15234375" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="5" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="5" collapsed="1"/>
+    <col min="5" max="5" width="24" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3569,111 +3355,111 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>332</v>
+        <v>261</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>244</v>
+        <v>190</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>333</v>
+        <v>262</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>245</v>
+        <v>191</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>334</v>
+        <v>263</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>246</v>
+        <v>192</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>335</v>
+        <v>264</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>247</v>
+        <v>193</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
-  <dimension ref="A1:M7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB9BADB-29CB-4747-93B5-EAB1AD94407A}">
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.84375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.15234375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.84375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.3828125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.69140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.84375" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.15234375" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3711,12 +3497,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>200</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3729,12 +3515,12 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>272</v>
+        <v>201</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3747,12 +3533,12 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>273</v>
+        <v>202</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3765,12 +3551,12 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3783,12 +3569,12 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>275</v>
+        <v>204</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -3801,12 +3587,12 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>276</v>
+        <v>205</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -3820,7 +3606,7 @@
       <c r="I7" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3828,23 +3614,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A029BA7-3086-406C-A77E-58AC14E2F6FE}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.15234375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.84375" collapsed="true"/>
-    <col min="3" max="4" style="1" width="9.15234375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.15234375" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.15234375" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3861,12 +3647,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>318</v>
+        <v>247</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3875,12 +3661,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>319</v>
+        <v>248</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3889,12 +3675,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>320</v>
+        <v>249</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3903,12 +3689,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>321</v>
+        <v>250</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3918,8 +3704,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3927,19 +3713,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B88DB0-56A9-4751-A2AB-F86F5E9F992C}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="1" width="14.84375" collapsed="true"/>
+    <col min="1" max="16384" width="14.85546875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3956,12 +3742,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>322</v>
+        <v>251</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3970,12 +3756,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>252</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3984,12 +3770,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>253</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3998,12 +3784,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>325</v>
+        <v>254</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -4013,8 +3799,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4022,31 +3808,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5C51F8-B59C-42E8-82FD-350399CB099A}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.84375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.84375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.15234375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.84375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.3828125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.69140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.84375" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.15234375" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4084,12 +3870,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>197</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -4102,12 +3888,12 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>269</v>
+        <v>198</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -4120,12 +3906,12 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>270</v>
+        <v>199</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -4138,7 +3924,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4146,25 +3932,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92052058-09B3-4B5F-984B-5ED260F80AB1}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.84375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="22.15234375" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.15234375" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4184,12 +3970,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>290</v>
+        <v>219</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -4201,12 +3987,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>291</v>
+        <v>220</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -4218,12 +4004,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>292</v>
+        <v>221</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -4236,8 +4022,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4245,25 +4031,25 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91231D0-74A2-4955-BD46-A8F29393EF1C}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.84375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.84375" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.15234375" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4283,12 +4069,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>289</v>
+        <v>218</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -4301,8 +4087,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4310,27 +4096,27 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.84375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="13.84375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.69140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.3828125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="19.3828125" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="19.42578125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4356,29 +4142,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>206</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>207</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -4390,29 +4176,29 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>279</v>
+        <v>208</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>280</v>
+        <v>209</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -4424,12 +4210,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>281</v>
+        <v>210</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -4441,12 +4227,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>282</v>
+        <v>211</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -4458,12 +4244,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>283</v>
+        <v>212</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -4475,12 +4261,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>284</v>
+        <v>213</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -4492,12 +4278,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>285</v>
+        <v>214</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -4509,12 +4295,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>286</v>
+        <v>215</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -4526,12 +4312,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -4543,12 +4329,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>288</v>
+        <v>217</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -4561,8 +4347,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -4570,31 +4356,31 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
-  <dimension ref="A1:M17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BF1DC6-8140-4BB0-A2E7-1959BCD7413E}">
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="47.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.69140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.3046875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="18.3046875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="19.84375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="20.53515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="23.84375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="36.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="35.3828125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.84375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="45.53515625" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="47.53515625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="36" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="35.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="45.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16384" width="47.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4632,12 +4418,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>48</v>
@@ -4664,12 +4450,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>48</v>
@@ -4696,12 +4482,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>48</v>
@@ -4728,12 +4514,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>23</v>
@@ -4760,15 +4546,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>46</v>
@@ -4789,18 +4575,18 @@
         <v>14</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>46</v>
@@ -4812,27 +4598,27 @@
         <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="J7" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>46</v>
@@ -4844,27 +4630,27 @@
         <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>46</v>
@@ -4876,27 +4662,27 @@
         <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>46</v>
@@ -4908,27 +4694,27 @@
         <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>46</v>
@@ -4940,27 +4726,27 @@
         <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E12" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>46</v>
@@ -4972,33 +4758,33 @@
         <v>13</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>326</v>
+        <v>255</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="F13" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>47</v>
@@ -5007,72 +4793,72 @@
         <v>13</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>327</v>
+        <v>256</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="F14" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G14" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="J14" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="I13" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
-    <hyperlink r:id="rId2" ref="I12" xr:uid="{72B34BFC-1C06-4629-A7D1-00835E578F1C}"/>
-    <hyperlink r:id="rId3" ref="J12" xr:uid="{05843862-7C41-4D97-A198-1A33D27EECAF}"/>
-    <hyperlink r:id="rId4" ref="J13" xr:uid="{4B596713-18AE-4E73-886D-498F1C2E6C62}"/>
+    <hyperlink ref="I13" r:id="rId1" xr:uid="{3F9F44A8-9B34-41E9-BAB0-00A6C19D92F8}"/>
+    <hyperlink ref="I12" r:id="rId2" xr:uid="{72B34BFC-1C06-4629-A7D1-00835E578F1C}"/>
+    <hyperlink ref="J12" r:id="rId3" xr:uid="{05843862-7C41-4D97-A198-1A33D27EECAF}"/>
+    <hyperlink ref="J13" r:id="rId4" xr:uid="{4B596713-18AE-4E73-886D-498F1C2E6C62}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId5" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Added BWP SelIDE Test Cases, Fixed VRelay 2.5 Issues
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F360F8C9-925E-4E3C-8B12-D64FEE1658F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93620B92-E472-40DC-9EBF-C74D31721CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
+    <workbookView xWindow="33450" yWindow="2805" windowWidth="15330" windowHeight="11490" firstSheet="5" activeTab="7" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" sheetId="1" r:id="rId1"/>
@@ -1241,7 +1241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E041308-6561-4EE5-9DD4-5DDA2695E487}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -4099,8 +4099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated UM-TestSuite-QA with Thread.Sleep
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/UM-Data.xlsx
+++ b/KatalonData/Bootstrap/UM-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t465179\Documents\git\VPS-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{93620B92-E472-40DC-9EBF-C74D31721CD2}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{EA277805-DA4E-4C09-9934-C13F3828E3AD}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="7" firstSheet="5" windowHeight="11490" windowWidth="15330" xWindow="33450" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="2805"/>
+    <workbookView activeTab="14" firstSheet="11" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{354FC140-4496-4D7F-AB69-566E59F6C646}" yWindow="-110"/>
   </bookViews>
   <sheets>
     <sheet name="CreateUser" r:id="rId1" sheetId="1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="350">
   <si>
     <t>Result</t>
   </si>
@@ -550,45 +550,9 @@
     <t>Minjas</t>
   </si>
   <si>
-    <t>username2371</t>
-  </si>
-  <si>
-    <t>Thu Sep 28 12:53:24 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Sep 28 12:53:54 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Sep 28 12:54:20 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Sep 28 12:54:41 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Sep 28 12:55:07 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Sep 28 12:55:33 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Sep 28 12:55:55 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Sep 28 12:56:20 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Sep 28 12:56:44 EDT 2023</t>
-  </si>
-  <si>
-    <t>Thu Sep 28 12:57:09 EDT 2023</t>
-  </si>
-  <si>
     <t>Username@12347</t>
   </si>
   <si>
-    <t>Thu Sep 28 13:40:32 EDT 2023</t>
-  </si>
-  <si>
     <t>username2439</t>
   </si>
   <si>
@@ -637,436 +601,508 @@
     <t>lancho</t>
   </si>
   <si>
-    <t>Fri Jul 12 18:51:44 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:52:20 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:52:52 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:53:24 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:53:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:54:25 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:54:56 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:55:19 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:55:42 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:56:04 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:56:27 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:56:50 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:57:13 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:57:43 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:58:09 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:58:35 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:59:03 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:59:27 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 18:59:53 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:00:19 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:00:46 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:01:14 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:01:39 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:02:05 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:02:31 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:02:40 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:02:55 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:03:10 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:03:26 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:03:55 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:04:25 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:04:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:05:24 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:05:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:06:24 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:06:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:07:24 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:07:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:08:23 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:08:53 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:09:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:09:53 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:10:22 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:10:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:12:49 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:13:21 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:13:53 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:14:25 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:14:57 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:15:28 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:15:55 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:16:28 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:17:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:17:49 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:18:14 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:18:36 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:18:58 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:19:21 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:19:45 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:20:07 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:20:30 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:20:54 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:21:16 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:22:46 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:23:14 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:23:40 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:24:06 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:24:32 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:24:57 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:25:19 EDT 2024</t>
-  </si>
-  <si>
-    <t>Fri Jul 12 19:25:41 EDT 2024</t>
+    <t>Sat Aug 16 18:37:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 18:37:22 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 18:37:32 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 18:37:41 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 18:37:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 18:38:01 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 18:42:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 18:42:37 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 18:42:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 18:58:52 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 18:59:04 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 18:59:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 18:59:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:22:02 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:22:18 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:24:26 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:31:53 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:32:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:32:59 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:45:04 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:45:18 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:45:31 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:45:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:45:59 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:46:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:46:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:46:37 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:46:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:47:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:47:18 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:47:31 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:48:57 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:51:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:51:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:52:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:52:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:53:21 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:53:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:54:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:54:58 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:55:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:56:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:56:30 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:57:02 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:57:32 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:58:02 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:58:32 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 19:59:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:16:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:17:10 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:17:38 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:18:02 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:18:26 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:18:53 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:19:17 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:23:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:24:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:26:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:26:35 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:26:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:27:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:28:33 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:28:54 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:29:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:29:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:31:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:31:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:32:06 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:32:26 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:32:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:33:26 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:33:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:34:05 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:34:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:34:44 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:35:24 EDT 2025</t>
+  </si>
+  <si>
+    <t>username23710</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:38:05 EDT 2025</t>
+  </si>
+  <si>
+    <t>Possible Defect Investigate</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:39:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:47:02 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:47:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:48:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:48:57 EDT 2025</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Wed Mar 26 19:17:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:41:30 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:42:16 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:42:50 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:43:19 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:43:46 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:44:14 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:44:42 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:45:01 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:45:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:45:40 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:45:59 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:46:18 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:46:37 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:46:59 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:47:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:47:42 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:48:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:48:28 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:48:52 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:49:14 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:49:35 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:49:59 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:50:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:50:43 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:51:08 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:51:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:51:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:51:52 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:52:10 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:52:37 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:53:05 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:53:33 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:53:59 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:54:29 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:54:55 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:55:23 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:55:51 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:56:22 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:56:51 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:57:18 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:57:45 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:58:12 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:58:40 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 22:59:09 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:01:02 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:01:27 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:01:55 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:02:24 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:02:52 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:03:24 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:03:48 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:04:16 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:04:49 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:05:25 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:05:50 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:06:10 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:06:30 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:06:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:07:12 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:07:31 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:07:55 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:08:14 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:08:34 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:09:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:10:24 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:10:54 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:11:19 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:11:45 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:12:13 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:12:34 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Apr 30 23:12:56 IST 2025</t>
+    <t>Sat Aug 16 21:52:08 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:52:57 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:53:44 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:54:32 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:56:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:57:30 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:58:07 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:58:39 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:59:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 21:59:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:00:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:00:30 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:00:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:00:59 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:01:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:01:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:01:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:02:05 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:02:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:02:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:02:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:03:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:03:17 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:03:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:03:50 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:04:05 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:04:21 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:04:35 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:04:50 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:05:02 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:05:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:05:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:05:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:06:18 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:07:19 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:07:54 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:08:35 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:09:10 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:09:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:10:21 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:10:56 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:11:31 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:12:07 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:12:42 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:13:17 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:13:52 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:14:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:15:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:15:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:16:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:16:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:17:04 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:17:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:17:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:18:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:18:38 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:19:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:20:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:20:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:20:56 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:21:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:21:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:21:56 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:22:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:22:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:22:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:23:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:23:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:23:54 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:24:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:24:35 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:24:54 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:25:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:25:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:25:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:27:08 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:27:53 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:28:40 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:29:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:30:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:30:23 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:30:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Sat Aug 16 22:30:45 EDT 2025</t>
   </si>
 </sst>
 </file>
@@ -1465,23 +1501,23 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.26953125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="14.1796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.81640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.453125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="26.7265625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="23.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="29.1796875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.81640625" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1516,12 +1552,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -1542,12 +1578,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1568,12 +1604,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -1611,18 +1647,18 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.1796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.26953125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="16.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="10.1796875" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="16.26953125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1642,7 +1678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1659,7 +1695,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1676,7 +1712,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1693,7 +1729,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1710,7 +1746,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1727,7 +1763,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1744,7 +1780,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1761,7 +1797,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1778,7 +1814,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1795,7 +1831,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1812,7 +1848,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1829,7 +1865,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -1846,7 +1882,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1863,7 +1899,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1880,7 +1916,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1897,7 +1933,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1914,7 +1950,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -1931,7 +1967,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1948,7 +1984,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1965,7 +2001,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -1982,7 +2018,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1999,7 +2035,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2016,7 +2052,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2033,7 +2069,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -2050,7 +2086,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -2067,7 +2103,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2084,7 +2120,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2101,7 +2137,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2118,7 +2154,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -2135,7 +2171,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -2152,7 +2188,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -2169,7 +2205,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -2186,7 +2222,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -2203,7 +2239,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -2220,7 +2256,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -2237,7 +2273,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -2254,7 +2290,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -2271,7 +2307,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2288,7 +2324,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -2305,7 +2341,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -2338,14 +2374,14 @@
       <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.26953125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2359,7 +2395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2370,7 +2406,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -2381,7 +2417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -2392,7 +2428,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -2403,7 +2439,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -2414,7 +2450,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -2425,7 +2461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -2436,7 +2472,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2447,7 +2483,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -2458,7 +2494,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -2469,7 +2505,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2480,7 +2516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -2491,7 +2527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2502,7 +2538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -2513,7 +2549,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2524,7 +2560,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2535,7 +2571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -2546,7 +2582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -2557,7 +2593,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2568,7 +2604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -2579,7 +2615,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -2590,7 +2626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2601,7 +2637,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2612,7 +2648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -2623,7 +2659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -2634,7 +2670,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2645,7 +2681,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2656,7 +2692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2667,7 +2703,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -2678,7 +2714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -2699,29 +2735,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BBB4B9-A457-4811-8CDB-D2D99106F229}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="1" width="28.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="38.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="38.26953125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="1" width="21.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="21.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="21.26953125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.81640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.453125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="26.7265625" collapsed="true"/>
     <col min="11" max="11" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
-    <col min="14" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="16.7265625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="12.7265625" collapsed="true"/>
+    <col min="14" max="16384" style="1" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2762,12 +2798,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>130</v>
@@ -2783,12 +2819,12 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row ht="30" r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>130</v>
@@ -2804,12 +2840,12 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row ht="30" r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>130</v>
@@ -2824,12 +2860,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>130</v>
@@ -2844,12 +2880,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>130</v>
@@ -2864,12 +2900,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>130</v>
@@ -2884,12 +2920,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>130</v>
@@ -2904,12 +2940,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>130</v>
@@ -2924,12 +2960,12 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="30" r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>130</v>
@@ -2944,12 +2980,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>130</v>
@@ -2964,12 +3000,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>130</v>
@@ -2984,12 +3020,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>130</v>
@@ -3004,12 +3040,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>130</v>
@@ -3024,12 +3060,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>130</v>
@@ -3044,12 +3080,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row ht="29" r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>130</v>
@@ -3064,12 +3100,12 @@
         <v>10</v>
       </c>
     </row>
-    <row ht="30" r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row ht="29" r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>130</v>
@@ -3096,26 +3132,26 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.26953125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="29.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="14.1796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.81640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.453125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="26.7265625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="23.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="29.1796875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.81640625" collapsed="true"/>
+    <col min="12" max="16384" style="1" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3150,12 +3186,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3176,12 +3212,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3215,20 +3251,20 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="19.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7265625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="19.453125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="22.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="22.54296875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.81640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.7265625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.453125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="19.453125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3260,15 +3296,15 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3286,12 +3322,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3309,12 +3345,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3332,12 +3368,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3355,12 +3391,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -3378,15 +3414,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -3404,12 +3440,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -3436,21 +3472,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A53983D-C89C-4548-8A02-C36CB8EC5C28}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="29.85546875" collapsed="true"/>
-    <col min="3" max="4" style="5" width="9.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="18.42578125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="29.81640625" collapsed="true"/>
+    <col min="3" max="4" style="5" width="9.1796875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="18.453125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="5" width="21.0" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3464,75 +3500,75 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>27</v>
@@ -3551,17 +3587,17 @@
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="22.7109375" collapsed="true"/>
-    <col min="3" max="4" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" style="5" width="9.1796875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="22.7265625" collapsed="true"/>
+    <col min="3" max="4" style="5" width="9.1796875" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="5" width="24.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="5" width="22.7109375" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="22.7265625" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3575,75 +3611,75 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>337</v>
+        <v>349</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>30</v>
@@ -3662,24 +3698,24 @@
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.81640625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.1796875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.81640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.453125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="26.7265625" collapsed="true"/>
     <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7265625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.81640625" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3717,12 +3753,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3735,12 +3771,12 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3753,12 +3789,12 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3771,12 +3807,12 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3789,12 +3825,12 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -3807,12 +3843,12 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -3841,16 +3877,16 @@
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="4" style="1" width="9.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.140625" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" style="1" width="9.1796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.81640625" collapsed="true"/>
+    <col min="3" max="4" style="1" width="9.1796875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.1796875" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3867,12 +3903,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3881,12 +3917,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3895,12 +3931,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -3909,12 +3945,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -3940,12 +3976,12 @@
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" style="1" width="14.85546875" collapsed="true"/>
+    <col min="1" max="16384" style="1" width="14.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3962,12 +3998,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -3976,12 +4012,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -3990,12 +4026,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -4004,12 +4040,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -4035,24 +4071,24 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.81640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.81640625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.1796875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="9.81640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.453125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="26.7265625" collapsed="true"/>
     <col min="10" max="10" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="16.7265625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="4.81640625" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4090,12 +4126,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -4108,12 +4144,12 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -4126,12 +4162,12 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -4159,18 +4195,18 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.26953125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="22.140625" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.1796875" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4190,12 +4226,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -4207,12 +4243,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -4224,12 +4260,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -4258,18 +4294,18 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.26953125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
-    <col min="7" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.81640625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4289,12 +4325,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -4319,24 +4355,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7D96D8-F32A-42CB-8719-B4A22D28EC0D}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="19.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.26953125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="19.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.81640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.7265625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.453125" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="19.453125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4362,29 +4398,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -4396,29 +4432,29 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -4430,12 +4466,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -4447,12 +4483,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -4464,12 +4500,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -4481,12 +4517,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -4498,12 +4534,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -4515,12 +4551,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -4532,12 +4568,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -4549,12 +4585,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -4580,27 +4616,27 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="47.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="47.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="26.7265625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="14.36328125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="19.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="18.26953125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="19.81640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="20.54296875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="23.81640625" collapsed="true"/>
     <col min="9" max="9" customWidth="true" style="1" width="36.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="35.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="45.5703125" collapsed="true"/>
-    <col min="13" max="16384" style="1" width="47.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="35.453125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="4.81640625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="45.54296875" collapsed="true"/>
+    <col min="13" max="16384" style="1" width="47.54296875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4638,12 +4674,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>332</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>48</v>
@@ -4670,12 +4709,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>333</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>48</v>
@@ -4702,12 +4744,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>334</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>48</v>
@@ -4734,12 +4779,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>335</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>23</v>
@@ -4766,12 +4814,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>336</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>150</v>
@@ -4798,15 +4849,18 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row ht="29" r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>259</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>165</v>
+        <v>258</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>46</v>
@@ -4817,7 +4871,7 @@
       <c r="H7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="4" t="s">
         <v>152</v>
       </c>
       <c r="J7" t="s">
@@ -4830,12 +4884,15 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>337</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>157</v>
@@ -4862,12 +4919,15 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>338</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>158</v>
@@ -4894,12 +4954,15 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>174</v>
+        <v>339</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>159</v>
@@ -4926,12 +4989,15 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>340</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>160</v>
@@ -4958,15 +5024,18 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>177</v>
+        <v>341</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>46</v>
@@ -4978,10 +5047,10 @@
         <v>13</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>14</v>
@@ -4990,21 +5059,21 @@
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row ht="29" r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>328</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>261</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F13" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>47</v>
@@ -5013,10 +5082,10 @@
         <v>13</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>14</v>
@@ -5025,18 +5094,18 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row ht="29" r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>329</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>257</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="F14" t="s">
         <v>164</v>
@@ -5060,13 +5129,13 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B16"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17"/>
     </row>
   </sheetData>
@@ -5076,9 +5145,10 @@
     <hyperlink r:id="rId2" ref="I12" xr:uid="{72B34BFC-1C06-4629-A7D1-00835E578F1C}"/>
     <hyperlink r:id="rId3" ref="J12" xr:uid="{05843862-7C41-4D97-A198-1A33D27EECAF}"/>
     <hyperlink r:id="rId4" ref="J13" xr:uid="{4B596713-18AE-4E73-886D-498F1C2E6C62}"/>
+    <hyperlink r:id="rId5" ref="I7" xr:uid="{03AFAD0B-8C1E-4C88-9D19-59B6814BCD72}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId5" verticalDpi="0"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId6" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>